<commit_message>
Cleaned up some more spreadsheets and some naming convention issues.
</commit_message>
<xml_diff>
--- a/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/BondTransactionPricer.xlsx
+++ b/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/BondTransactionPricer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2017\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Product Pricers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2019\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Product Pricers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D5C15E-9467-4145-8703-A3916064B497}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4114AEB-0FAC-4254-8214-513C5B8D05F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="18075" windowHeight="12270" tabRatio="836" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="0" windowWidth="26370" windowHeight="14820" tabRatio="836" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AUDDiscountCurve" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,15 @@
     <definedName name="Rates" localSheetId="0">AUDDiscountCurve!$D$18:$D$41</definedName>
     <definedName name="Spreads" localSheetId="0">AUDDiscountCurve!$E$18:$E$41</definedName>
   </definedNames>
-  <calcPr calcId="179017" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2183,7 +2191,7 @@
       <c r="F1" s="81"/>
       <c r="G1" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G2:H12, $C$18:$E$41)</f>
-        <v>Market.QR_LIVE.2018-04-25.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-06-25.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H1" s="122"/>
       <c r="I1" s="81"/>
@@ -2213,7 +2221,7 @@
       </c>
       <c r="B3" s="85">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="C3" s="80"/>
       <c r="D3" s="80"/>
@@ -2224,7 +2232,7 @@
       </c>
       <c r="H3" s="85">
         <f ca="1">H6</f>
-        <v>43215</v>
+        <v>43641</v>
       </c>
       <c r="I3" s="84"/>
     </row>
@@ -2234,7 +2242,7 @@
       </c>
       <c r="B4" s="86">
         <f ca="1">B3</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="C4" s="80"/>
       <c r="D4" s="80"/>
@@ -2245,7 +2253,7 @@
       </c>
       <c r="H4" s="86">
         <f ca="1">H3</f>
-        <v>43215</v>
+        <v>43641</v>
       </c>
       <c r="I4" s="84"/>
     </row>
@@ -2284,7 +2292,7 @@
       </c>
       <c r="H6" s="88">
         <f ca="1">'BondCurve-BondForward'!G7</f>
-        <v>43215</v>
+        <v>43641</v>
       </c>
       <c r="I6" s="84"/>
     </row>
@@ -2429,7 +2437,7 @@
       <c r="F14" s="84"/>
       <c r="G14" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G15:H25,HLInstruments)</f>
-        <v>Market.QR_LIVE.2018-04-24.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-06-24.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H14" s="122"/>
       <c r="I14" s="84"/>
@@ -2463,7 +2471,7 @@
       </c>
       <c r="H16" s="85">
         <f ca="1">H19</f>
-        <v>43214</v>
+        <v>43640</v>
       </c>
       <c r="I16" s="84"/>
     </row>
@@ -2489,7 +2497,7 @@
       </c>
       <c r="H17" s="86">
         <f ca="1">H16</f>
-        <v>43214</v>
+        <v>43640</v>
       </c>
       <c r="I17" s="84"/>
     </row>
@@ -2542,7 +2550,7 @@
       </c>
       <c r="H19" s="88">
         <f ca="1">'BondCurve-BondForward'!G21</f>
-        <v>43214</v>
+        <v>43640</v>
       </c>
       <c r="I19" s="84"/>
     </row>
@@ -2744,7 +2752,7 @@
       <c r="F27" s="84"/>
       <c r="G27" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G28:H38, HLInstruments)</f>
-        <v>Market.QR_LIVE.2018-04-23.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-06-23.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H27" s="122"/>
       <c r="I27" s="84"/>
@@ -2798,7 +2806,7 @@
       </c>
       <c r="H29" s="85">
         <f ca="1">H32</f>
-        <v>43213</v>
+        <v>43639</v>
       </c>
       <c r="I29" s="84"/>
     </row>
@@ -2825,7 +2833,7 @@
       </c>
       <c r="H30" s="86">
         <f ca="1">H29</f>
-        <v>43213</v>
+        <v>43639</v>
       </c>
       <c r="I30" s="84"/>
     </row>
@@ -2878,7 +2886,7 @@
       </c>
       <c r="H32" s="88">
         <f ca="1">'BondCurve-BondForward'!G35</f>
-        <v>43213</v>
+        <v>43639</v>
       </c>
       <c r="I32" s="84"/>
     </row>
@@ -3080,7 +3088,7 @@
       <c r="F40" s="84"/>
       <c r="G40" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G41:H51, HLInstruments)</f>
-        <v>Market.QR_LIVE.2018-04-22.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-06-22.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H40" s="122"/>
       <c r="I40" s="84"/>
@@ -3123,7 +3131,7 @@
       </c>
       <c r="H42" s="85">
         <f ca="1">H45</f>
-        <v>43212</v>
+        <v>43638</v>
       </c>
       <c r="I42" s="84"/>
     </row>
@@ -3141,7 +3149,7 @@
       </c>
       <c r="H43" s="86">
         <f ca="1">H42</f>
-        <v>43212</v>
+        <v>43638</v>
       </c>
       <c r="I43" s="84"/>
     </row>
@@ -3172,7 +3180,7 @@
       </c>
       <c r="H45" s="88">
         <f ca="1">'BondCurve-BondForward'!G49</f>
-        <v>43212</v>
+        <v>43638</v>
       </c>
       <c r="I45" s="82"/>
     </row>
@@ -3229,7 +3237,7 @@
     <row r="53" spans="7:8" ht="13.5" thickBot="1">
       <c r="G53" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G54:H64, HLInstruments)</f>
-        <v>Market.QR_LIVE.2018-04-21.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-06-21.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H53" s="122"/>
     </row>
@@ -3247,7 +3255,7 @@
       </c>
       <c r="H55" s="85">
         <f ca="1">H58</f>
-        <v>43211</v>
+        <v>43637</v>
       </c>
     </row>
     <row r="56" spans="7:8">
@@ -3256,7 +3264,7 @@
       </c>
       <c r="H56" s="86">
         <f ca="1">H55</f>
-        <v>43211</v>
+        <v>43637</v>
       </c>
     </row>
     <row r="57" spans="7:8">
@@ -3273,7 +3281,7 @@
       </c>
       <c r="H58" s="88">
         <f ca="1">'BondCurve-BondForward'!G63</f>
-        <v>43211</v>
+        <v>43637</v>
       </c>
     </row>
     <row r="59" spans="7:8">
@@ -3398,7 +3406,7 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -3407,7 +3415,7 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -3680,7 +3688,7 @@
       </c>
       <c r="C39" s="31">
         <f ca="1"/>
-        <v>2.4999999999999991E-2</v>
+        <v>2.5000000000000012E-2</v>
       </c>
     </row>
     <row r="40" spans="2:3">
@@ -3747,14 +3755,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F58" sqref="F58:G58"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="61" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
@@ -3770,7 +3778,7 @@
       <c r="C2" s="124"/>
       <c r="F2" s="123" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F3:G15, $B$18:$D$21)</f>
-        <v>Market.QR_LIVE.2018-04-25.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-06-25.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G2" s="124"/>
     </row>
@@ -3794,14 +3802,14 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="25">
         <f ca="1">G7</f>
-        <v>43215</v>
+        <v>43641</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -3810,14 +3818,14 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="26">
         <f ca="1">G4</f>
-        <v>43215</v>
+        <v>43641</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -3835,7 +3843,7 @@
       </c>
       <c r="I6" t="str">
         <f ca="1">G6&amp;"."&amp;TEXT(G7,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2018-04-25</v>
+        <v>QR_LIVE.2019-06-25</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -3850,11 +3858,11 @@
       </c>
       <c r="G7" s="77">
         <f ca="1">$C$5-1</f>
-        <v>43215</v>
+        <v>43641</v>
       </c>
       <c r="I7" t="str">
         <f ca="1">G20&amp;"."&amp;TEXT(G21,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2018-04-24</v>
+        <v>QR_LIVE.2019-06-24</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -3872,7 +3880,7 @@
       </c>
       <c r="I8" t="str">
         <f ca="1">G34&amp;"."&amp;TEXT(G35,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2018-04-23</v>
+        <v>QR_LIVE.2019-06-23</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -3890,7 +3898,7 @@
       </c>
       <c r="I9" t="str">
         <f ca="1">G48&amp;"."&amp;TEXT(G49,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2018-04-22</v>
+        <v>QR_LIVE.2019-06-22</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -3908,7 +3916,7 @@
       </c>
       <c r="I10" t="str">
         <f ca="1">G62&amp;"."&amp;TEXT(G63,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2018-04-21</v>
+        <v>QR_LIVE.2019-06-21</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -3981,7 +3989,7 @@
       <c r="D16" s="13"/>
       <c r="F16" s="125" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F17:G29, $B$23:$D$26)</f>
-        <v>Market.QR_LIVE.2018-04-24.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-06-24.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G16" s="126"/>
     </row>
@@ -4017,7 +4025,7 @@
       </c>
       <c r="G18" s="25">
         <f ca="1">G21</f>
-        <v>43214</v>
+        <v>43640</v>
       </c>
     </row>
     <row r="19" spans="2:7">
@@ -4035,7 +4043,7 @@
       </c>
       <c r="G19" s="26">
         <f ca="1">G18</f>
-        <v>43214</v>
+        <v>43640</v>
       </c>
     </row>
     <row r="20" spans="2:7">
@@ -4071,7 +4079,7 @@
       </c>
       <c r="G21" s="77">
         <f ca="1">$G$7-1</f>
-        <v>43214</v>
+        <v>43640</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="13.5" thickBot="1">
@@ -4204,7 +4212,7 @@
       </c>
       <c r="F30" s="125" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F31:G43, $B$28:$D$31)</f>
-        <v>Market.QR_LIVE.2018-04-23.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-06-23.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G30" s="126"/>
     </row>
@@ -4231,7 +4239,7 @@
       </c>
       <c r="G32" s="25">
         <f ca="1">G35</f>
-        <v>43213</v>
+        <v>43639</v>
       </c>
     </row>
     <row r="33" spans="2:7">
@@ -4249,7 +4257,7 @@
       </c>
       <c r="G33" s="26">
         <f ca="1">G32</f>
-        <v>43213</v>
+        <v>43639</v>
       </c>
     </row>
     <row r="34" spans="2:7">
@@ -4285,7 +4293,7 @@
       </c>
       <c r="G35" s="77">
         <f ca="1">$G$7-2</f>
-        <v>43213</v>
+        <v>43639</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="13.5" thickBot="1">
@@ -4403,7 +4411,7 @@
       </c>
       <c r="F44" s="125" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F45:G57, $B$33:$D$36)</f>
-        <v>Market.QR_LIVE.2018-04-22.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-06-22.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G44" s="126"/>
     </row>
@@ -4437,7 +4445,7 @@
       </c>
       <c r="G46" s="25">
         <f ca="1">G49</f>
-        <v>43212</v>
+        <v>43638</v>
       </c>
     </row>
     <row r="47" spans="2:7">
@@ -4454,7 +4462,7 @@
       </c>
       <c r="G47" s="26">
         <f ca="1">G46</f>
-        <v>43212</v>
+        <v>43638</v>
       </c>
     </row>
     <row r="48" spans="2:7">
@@ -4488,7 +4496,7 @@
       </c>
       <c r="G49" s="77">
         <f ca="1">$G$7-3</f>
-        <v>43212</v>
+        <v>43638</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="13.5" thickBot="1">
@@ -4513,7 +4521,7 @@
     <row r="52" spans="2:7">
       <c r="B52" s="73">
         <f t="array" aca="1" ref="B52:C56" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="C52" s="30">
         <f ca="1"/>
@@ -4529,7 +4537,7 @@
     <row r="53" spans="2:7">
       <c r="B53" s="74">
         <f ca="1"/>
-        <v>43220</v>
+        <v>43644</v>
       </c>
       <c r="C53" s="31">
         <f ca="1"/>
@@ -4545,7 +4553,7 @@
     <row r="54" spans="2:7">
       <c r="B54" s="74">
         <f ca="1"/>
-        <v>43250</v>
+        <v>43675</v>
       </c>
       <c r="C54" s="31">
         <f ca="1"/>
@@ -4561,7 +4569,7 @@
     <row r="55" spans="2:7">
       <c r="B55" s="74">
         <f ca="1"/>
-        <v>43283</v>
+        <v>43705</v>
       </c>
       <c r="C55" s="31">
         <f ca="1"/>
@@ -4604,14 +4612,14 @@
       </c>
       <c r="F58" s="125" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F59:G71, $B$38:$D$41)</f>
-        <v>Market.QR_LIVE.2018-04-21.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-06-21.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G58" s="126"/>
     </row>
     <row r="59" spans="2:7" ht="13.5" thickBot="1">
       <c r="B59" s="73">
         <f ca="1">B52</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="C59" s="30">
         <f t="array" aca="1" ref="C59:C63" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B52:B56)</f>
@@ -4627,7 +4635,7 @@
     <row r="60" spans="2:7">
       <c r="B60" s="74">
         <f t="shared" ref="B60:B63" ca="1" si="0">B53</f>
-        <v>43220</v>
+        <v>43644</v>
       </c>
       <c r="C60" s="31">
         <f ca="1"/>
@@ -4638,34 +4646,34 @@
       </c>
       <c r="G60" s="25">
         <f ca="1">G63</f>
-        <v>43211</v>
+        <v>43637</v>
       </c>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43250</v>
+        <v>43675</v>
       </c>
       <c r="C61" s="31">
         <f ca="1"/>
-        <v>4.9999999999999982E-2</v>
+        <v>5.000000000000001E-2</v>
       </c>
       <c r="F61" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G61" s="26">
         <f ca="1">G60</f>
-        <v>43211</v>
+        <v>43637</v>
       </c>
     </row>
     <row r="62" spans="2:7">
       <c r="B62" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43283</v>
+        <v>43705</v>
       </c>
       <c r="C62" s="31">
         <f ca="1"/>
-        <v>5.000000000000001E-2</v>
+        <v>4.9999999999999982E-2</v>
       </c>
       <c r="F62" s="22" t="s">
         <v>26</v>
@@ -4689,7 +4697,7 @@
       </c>
       <c r="G63" s="77">
         <f ca="1">$G$7-4</f>
-        <v>43211</v>
+        <v>43637</v>
       </c>
     </row>
     <row r="64" spans="2:7">
@@ -4807,7 +4815,7 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -4816,7 +4824,7 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -5024,7 +5032,7 @@
     <row r="32" spans="2:4">
       <c r="B32" s="73">
         <f t="array" aca="1" ref="B32:C36" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="C32" s="30">
         <f ca="1"/>
@@ -5034,7 +5042,7 @@
     <row r="33" spans="2:3">
       <c r="B33" s="74">
         <f ca="1"/>
-        <v>43217</v>
+        <v>43643</v>
       </c>
       <c r="C33" s="31">
         <f ca="1"/>
@@ -5044,17 +5052,17 @@
     <row r="34" spans="2:3">
       <c r="B34" s="74">
         <f ca="1"/>
-        <v>43248</v>
+        <v>43675</v>
       </c>
       <c r="C34" s="31">
         <f ca="1"/>
-        <v>0.99563499344803497</v>
+        <v>0.99549920035018302</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="74">
         <f ca="1"/>
-        <v>43278</v>
+        <v>43704</v>
       </c>
       <c r="C35" s="31">
         <f ca="1"/>
@@ -5064,11 +5072,11 @@
     <row r="36" spans="2:3" ht="13.5" thickBot="1">
       <c r="B36" s="75">
         <f ca="1"/>
-        <v>43308</v>
+        <v>43735</v>
       </c>
       <c r="C36" s="32">
         <f ca="1"/>
-        <v>0.98755244716108004</v>
+        <v>0.98741884969798999</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="13.5" thickBot="1"/>
@@ -5080,7 +5088,7 @@
     <row r="39" spans="2:3">
       <c r="B39" s="73">
         <f ca="1">B32</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="C39" s="30">
         <f t="array" aca="1" ref="C39:C43" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B32:B36)</f>
@@ -5090,7 +5098,7 @@
     <row r="40" spans="2:3">
       <c r="B40" s="74">
         <f t="shared" ref="B40:B43" ca="1" si="0">B33</f>
-        <v>43217</v>
+        <v>43643</v>
       </c>
       <c r="C40" s="31">
         <f ca="1"/>
@@ -5100,17 +5108,17 @@
     <row r="41" spans="2:3">
       <c r="B41" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43248</v>
+        <v>43675</v>
       </c>
       <c r="C41" s="31">
         <f ca="1"/>
-        <v>0.99563499344803497</v>
+        <v>0.99549920035018302</v>
       </c>
     </row>
     <row r="42" spans="2:3">
       <c r="B42" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43278</v>
+        <v>43704</v>
       </c>
       <c r="C42" s="31">
         <f ca="1"/>
@@ -5120,11 +5128,11 @@
     <row r="43" spans="2:3" ht="13.5" thickBot="1">
       <c r="B43" s="75">
         <f t="shared" ca="1" si="0"/>
-        <v>43308</v>
+        <v>43735</v>
       </c>
       <c r="C43" s="32">
         <f ca="1"/>
-        <v>0.98755244716108015</v>
+        <v>0.9874188496979901</v>
       </c>
     </row>
     <row r="45" spans="2:3">
@@ -5212,14 +5220,14 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="25">
         <f ca="1">G5</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -5228,14 +5236,14 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -5443,7 +5451,7 @@
       </c>
       <c r="G20" s="25">
         <f ca="1">G21</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -5462,7 +5470,7 @@
       </c>
       <c r="G21" s="26">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="22" spans="2:7">
@@ -5563,7 +5571,7 @@
       </c>
       <c r="C28" s="65">
         <f ca="1"/>
-        <v>5.0018436500936764E-2</v>
+        <v>5.0006635273972595E-2</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>35</v>
@@ -5579,7 +5587,7 @@
       </c>
       <c r="C29" s="65">
         <f ca="1"/>
-        <v>5.0019491327740626E-2</v>
+        <v>5.0006741489319828E-2</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>37</v>
@@ -5595,7 +5603,7 @@
       </c>
       <c r="C30" s="65">
         <f ca="1"/>
-        <v>5.001988240740151E-2</v>
+        <v>5.0006799734284978E-2</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>38</v>
@@ -5642,7 +5650,7 @@
     <row r="34" spans="2:7" ht="13.5" thickBot="1">
       <c r="B34" s="73">
         <f t="array" aca="1" ref="B34:C38" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="C34" s="64">
         <f ca="1"/>
@@ -5657,7 +5665,7 @@
     <row r="35" spans="2:7" ht="13.5" thickBot="1">
       <c r="B35" s="74">
         <f ca="1"/>
-        <v>43217</v>
+        <v>43643</v>
       </c>
       <c r="C35" s="65">
         <f ca="1"/>
@@ -5673,45 +5681,45 @@
     <row r="36" spans="2:7">
       <c r="B36" s="74">
         <f ca="1"/>
-        <v>43248</v>
+        <v>43675</v>
       </c>
       <c r="C36" s="65">
         <f ca="1"/>
-        <v>0.99563344066314796</v>
+        <v>0.99549862334982497</v>
       </c>
       <c r="F36" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G36" s="25">
         <f ca="1">G37</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="74">
         <f ca="1"/>
-        <v>43278</v>
+        <v>43704</v>
       </c>
       <c r="C37" s="65">
         <f ca="1"/>
-        <v>0.99157404672121396</v>
+        <v>0.99157614205086997</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G37" s="26">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="13.5" thickBot="1">
       <c r="B38" s="75">
         <f ca="1"/>
-        <v>43308</v>
+        <v>43735</v>
       </c>
       <c r="C38" s="66">
         <f ca="1"/>
-        <v>0.98754761217961795</v>
+        <v>0.98741717842536103</v>
       </c>
       <c r="F38" s="22" t="s">
         <v>26</v>
@@ -5744,7 +5752,7 @@
     <row r="41" spans="2:7">
       <c r="B41" s="73">
         <f ca="1">B34</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="C41" s="64">
         <f t="array" aca="1" ref="C41:C45" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B34:B38)</f>
@@ -5760,7 +5768,7 @@
     <row r="42" spans="2:7">
       <c r="B42" s="74">
         <f t="shared" ref="B42:B45" ca="1" si="0">B35</f>
-        <v>43217</v>
+        <v>43643</v>
       </c>
       <c r="C42" s="65">
         <f ca="1"/>
@@ -5776,11 +5784,11 @@
     <row r="43" spans="2:7">
       <c r="B43" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43248</v>
+        <v>43675</v>
       </c>
       <c r="C43" s="65">
         <f ca="1"/>
-        <v>5.0227865084556497E-2</v>
+        <v>5.0212902395297299E-2</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>34</v>
@@ -5792,11 +5800,11 @@
     <row r="44" spans="2:7">
       <c r="B44" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43278</v>
+        <v>43704</v>
       </c>
       <c r="C44" s="65">
         <f ca="1"/>
-        <v>5.0126043981842699E-2</v>
+        <v>5.0113447890619299E-2</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>35</v>
@@ -5808,11 +5816,11 @@
     <row r="45" spans="2:7" ht="13.5" thickBot="1">
       <c r="B45" s="75">
         <f t="shared" ca="1" si="0"/>
-        <v>43308</v>
+        <v>43735</v>
       </c>
       <c r="C45" s="66">
         <f ca="1"/>
-        <v>5.00238834529751E-2</v>
+        <v>5.0007532584952899E-2</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>37</v>
@@ -5884,7 +5892,7 @@
       </c>
       <c r="G52" s="25">
         <f ca="1">G53</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="53" spans="2:7">
@@ -5893,7 +5901,7 @@
       </c>
       <c r="G53" s="26">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="54" spans="2:7">
@@ -6011,7 +6019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -6129,7 +6137,7 @@
       </c>
       <c r="C10" s="2">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="G10" t="str">
         <v>AssetSwapSpread</v>
@@ -6141,7 +6149,7 @@
       </c>
       <c r="C11" s="2">
         <f ca="1">C10+5</f>
-        <v>43221</v>
+        <v>43647</v>
       </c>
       <c r="G11" t="str">
         <v>ZSpread</v>
@@ -6197,7 +6205,7 @@
       </c>
       <c r="C16" s="2">
         <f ca="1">C10</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="E16" t="str">
         <f t="array" aca="1" ref="E16:F22" ca="1">_xll.HLV5r3.Financial.Cache.ViewValuationReport(E28)</f>
@@ -6221,7 +6229,7 @@
       </c>
       <c r="F17" s="60">
         <f ca="1"/>
-        <v>-2.8896389690185529E-4</v>
+        <v>-1.97487625768998E-4</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -6237,7 +6245,7 @@
       </c>
       <c r="F18" s="115">
         <f ca="1"/>
-        <v>103007964.87326388</v>
+        <v>105500906.39820515</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -6253,7 +6261,7 @@
       </c>
       <c r="F19" s="115">
         <f ca="1"/>
-        <v>2064413.3926520003</v>
+        <v>4529812.7358730007</v>
       </c>
     </row>
     <row r="20" spans="2:6">
@@ -6269,7 +6277,7 @@
       </c>
       <c r="F20">
         <f ca="1"/>
-        <v>1.03064413392652</v>
+        <v>1.0552981273587301</v>
       </c>
     </row>
     <row r="21" spans="2:6">
@@ -6372,11 +6380,11 @@
       </c>
       <c r="E29" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F29,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2018-04-25</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-25</v>
       </c>
       <c r="F29" t="str">
         <f ca="1">'BondCurve-BondForward'!I6</f>
-        <v>QR_LIVE.2018-04-25</v>
+        <v>QR_LIVE.2019-06-25</v>
       </c>
     </row>
     <row r="30" spans="2:6">
@@ -6390,11 +6398,11 @@
       </c>
       <c r="E30" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F30,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2018-04-24</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-24</v>
       </c>
       <c r="F30" t="str">
         <f ca="1">'BondCurve-BondForward'!I7</f>
-        <v>QR_LIVE.2018-04-24</v>
+        <v>QR_LIVE.2019-06-24</v>
       </c>
     </row>
     <row r="31" spans="2:6">
@@ -6408,11 +6416,11 @@
       </c>
       <c r="E31" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F31,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2018-04-23</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-23</v>
       </c>
       <c r="F31" t="str">
         <f ca="1">'BondCurve-BondForward'!I8</f>
-        <v>QR_LIVE.2018-04-23</v>
+        <v>QR_LIVE.2019-06-23</v>
       </c>
     </row>
     <row r="32" spans="2:6">
@@ -6426,17 +6434,17 @@
       </c>
       <c r="E32" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F32,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2018-04-22</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-22</v>
       </c>
       <c r="F32" t="str">
         <f ca="1">'BondCurve-BondForward'!I9</f>
-        <v>QR_LIVE.2018-04-22</v>
+        <v>QR_LIVE.2019-06-22</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" t="str">
         <f ca="1"/>
-        <v>paryt1</v>
+        <v>party1</v>
       </c>
       <c r="C33" t="str">
         <f ca="1"/>
@@ -6444,11 +6452,11 @@
       </c>
       <c r="E33" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F33,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2018-04-21</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-21</v>
       </c>
       <c r="F33" t="str">
         <f ca="1">'BondCurve-BondForward'!I10</f>
-        <v>QR_LIVE.2018-04-21</v>
+        <v>QR_LIVE.2019-06-21</v>
       </c>
     </row>
     <row r="34" spans="2:6">
@@ -6584,8 +6592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:H55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6709,7 +6717,7 @@
       </c>
       <c r="C10" s="2">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="E10" s="114" t="s">
         <v>140</v>
@@ -6727,7 +6735,7 @@
       </c>
       <c r="C11" s="2">
         <f ca="1">C10+5</f>
-        <v>43221</v>
+        <v>43647</v>
       </c>
       <c r="H11" t="str">
         <v>ZSpread</v>
@@ -6783,7 +6791,7 @@
       </c>
       <c r="C16" s="2">
         <f ca="1">C10</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="E16" s="61" t="str">
         <f t="array" ref="E16:F22">_xll.HLV5r3.Financial.Cache.ViewValuationReport(E27)</f>
@@ -6957,7 +6965,7 @@
       </c>
       <c r="H29" s="1" t="str">
         <f t="array" aca="1" ref="H29:H33" ca="1">Markets</f>
-        <v>QR_LIVE.2018-04-25</v>
+        <v>QR_LIVE.2019-06-25</v>
       </c>
     </row>
     <row r="30" spans="2:8">
@@ -6971,7 +6979,7 @@
       </c>
       <c r="H30" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2018-04-24</v>
+        <v>QR_LIVE.2019-06-24</v>
       </c>
     </row>
     <row r="31" spans="2:8">
@@ -6985,7 +6993,7 @@
       </c>
       <c r="H31" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2018-04-23</v>
+        <v>QR_LIVE.2019-06-23</v>
       </c>
     </row>
     <row r="32" spans="2:8">
@@ -7006,27 +7014,27 @@
       </c>
       <c r="H32" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2018-04-22</v>
+        <v>QR_LIVE.2019-06-22</v>
       </c>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" t="str">
         <f ca="1"/>
-        <v>paryt1</v>
+        <v>party1</v>
       </c>
       <c r="C33" t="str">
         <f ca="1"/>
         <v>CBA</v>
       </c>
       <c r="E33" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_001.QR_LIVE.2018-02-21</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_001.QR_LIVE.2018-02-22</v>
       </c>
       <c r="F33" s="120">
         <v>0</v>
       </c>
       <c r="H33" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2018-04-21</v>
+        <v>QR_LIVE.2019-06-21</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -7039,10 +7047,10 @@
         <v>NAB</v>
       </c>
       <c r="E34" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_001.QR_LIVE.2018-02-20</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.bondTransaction.testtrade_002.QR_LIVE.2018-02-19</v>
       </c>
       <c r="F34" s="120">
-        <v>0</v>
+        <v>111644767.66734304</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -7055,10 +7063,10 @@
         <v>WATC 7 10/15/19</v>
       </c>
       <c r="E35" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_001.QR_LIVE.2018-02-19</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.bondTransaction.testtrade_002.QR_LIVE.2018-02-20</v>
       </c>
       <c r="F35" s="120">
-        <v>0</v>
+        <v>111709224.27935375</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -7071,10 +7079,10 @@
         <v>#N/A</v>
       </c>
       <c r="E36" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-23</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.bondTransaction.testtrade_002.QR_LIVE.2018-02-21</v>
       </c>
       <c r="F36" s="120">
-        <v>0</v>
+        <v>111868041.82686561</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -7087,7 +7095,7 @@
         <v>#N/A</v>
       </c>
       <c r="E37" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-22</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_001.QR_LIVE.2018-02-21</v>
       </c>
       <c r="F37" s="120">
         <v>0</v>
@@ -7103,7 +7111,7 @@
         <v>#N/A</v>
       </c>
       <c r="E38" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-21</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_001.QR_LIVE.2018-02-20</v>
       </c>
       <c r="F38" s="120">
         <v>0</v>
@@ -7119,7 +7127,7 @@
         <v>#N/A</v>
       </c>
       <c r="E39" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-20</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_001.QR_LIVE.2018-02-19</v>
       </c>
       <c r="F39" s="120">
         <v>0</v>
@@ -7135,7 +7143,7 @@
         <v>#N/A</v>
       </c>
       <c r="E40" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-19</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-23</v>
       </c>
       <c r="F40" s="120">
         <v>0</v>
@@ -7151,7 +7159,7 @@
         <v>#N/A</v>
       </c>
       <c r="E41" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_001.QR_LIVE.2018-02-22</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-22</v>
       </c>
       <c r="F41" s="120">
         <v>0</v>
@@ -7167,10 +7175,10 @@
         <v>#N/A</v>
       </c>
       <c r="E42" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.bondTransaction.testtrade_002.QR_LIVE.2018-02-19</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-21</v>
       </c>
       <c r="F42" s="120">
-        <v>111644767.66734304</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -7183,10 +7191,10 @@
         <v>#N/A</v>
       </c>
       <c r="E43" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.bondTransaction.testtrade_002.QR_LIVE.2018-02-20</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-20</v>
       </c>
       <c r="F43" s="120">
-        <v>111709224.27935375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -7199,10 +7207,10 @@
         <v>#N/A</v>
       </c>
       <c r="E44" t="str">
-        <v>ValuationReport.Var_Run_20170531.SpreadSheet.bondTransaction.testtrade_002.QR_LIVE.2018-02-21</v>
+        <v>ValuationReport.Var_Run_20170531.SpreadSheet.futureTransaction.testtrade_002.QR_LIVE.2018-02-19</v>
       </c>
       <c r="F44" s="120">
-        <v>111868041.82686561</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -7380,7 +7388,7 @@
       </c>
       <c r="K3" s="50">
         <f ca="1">TODAY()</f>
-        <v>43216</v>
+        <v>43642</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>21</v>
@@ -7489,11 +7497,11 @@
       </c>
       <c r="F7" s="2">
         <f ca="1">TODAY()-20</f>
-        <v>43196</v>
+        <v>43622</v>
       </c>
       <c r="G7" s="2">
         <f ca="1">F7+3</f>
-        <v>43199</v>
+        <v>43625</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>142</v>
@@ -7548,15 +7556,15 @@
       </c>
       <c r="R8" s="37">
         <f ca="1"/>
-        <v>-2.8896389690185529E-4</v>
+        <v>-1.97487625768998E-4</v>
       </c>
       <c r="S8" s="57">
         <f ca="1"/>
-        <v>103007.96487326389</v>
+        <v>105500.90639820514</v>
       </c>
       <c r="T8" s="57">
         <f ca="1"/>
-        <v>2064.4133926520003</v>
+        <v>4529.8127358729998</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -7577,11 +7585,11 @@
       </c>
       <c r="F9" s="2">
         <f ca="1">F7+2</f>
-        <v>43198</v>
+        <v>43624</v>
       </c>
       <c r="G9" s="2">
         <f ca="1">F9+3</f>
-        <v>43201</v>
+        <v>43627</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>142</v>
@@ -7644,15 +7652,15 @@
       </c>
       <c r="R10" s="37">
         <f ca="1"/>
-        <v>-2.8896389690185529E-4</v>
+        <v>-1.97487625768998E-4</v>
       </c>
       <c r="S10" s="57">
         <f ca="1"/>
-        <v>206015.92974652778</v>
+        <v>211001.81279641029</v>
       </c>
       <c r="T10" s="57">
         <f ca="1"/>
-        <v>4128.8267853040006</v>
+        <v>9059.6254717459997</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -7673,11 +7681,11 @@
       </c>
       <c r="F11" s="2">
         <f ca="1">F9+2</f>
-        <v>43200</v>
+        <v>43626</v>
       </c>
       <c r="G11" s="2">
         <f ca="1">F11+3</f>
-        <v>43203</v>
+        <v>43629</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>142</v>
@@ -7740,15 +7748,15 @@
       </c>
       <c r="R12" s="37">
         <f ca="1"/>
-        <v>-2.8896389690185529E-4</v>
+        <v>-1.97487625768998E-4</v>
       </c>
       <c r="S12" s="57">
         <f ca="1"/>
-        <v>309023.89461979165</v>
+        <v>316502.71919461543</v>
       </c>
       <c r="T12" s="57">
         <f ca="1"/>
-        <v>6193.2401779559996</v>
+        <v>13589.438207619001</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -7769,11 +7777,11 @@
       </c>
       <c r="F13" s="2">
         <f ca="1">F11+2</f>
-        <v>43202</v>
+        <v>43628</v>
       </c>
       <c r="G13" s="2">
         <f ca="1">F13+3</f>
-        <v>43205</v>
+        <v>43631</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>142</v>
@@ -7836,15 +7844,15 @@
       </c>
       <c r="R14" s="37">
         <f ca="1"/>
-        <v>0.14028896389690187</v>
+        <v>0.140197487625769</v>
       </c>
       <c r="S14" s="57">
         <f ca="1"/>
-        <v>-412031.85949305556</v>
+        <v>-422003.62559282058</v>
       </c>
       <c r="T14" s="57">
         <f ca="1"/>
-        <v>-8257.6535706079994</v>
+        <v>-18119.250943491999</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -7865,11 +7873,11 @@
       </c>
       <c r="F15" s="2">
         <f ca="1">F13+2</f>
-        <v>43204</v>
+        <v>43630</v>
       </c>
       <c r="G15" s="2">
         <f ca="1">F15+3</f>
-        <v>43207</v>
+        <v>43633</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>142</v>
@@ -7931,15 +7939,15 @@
       </c>
       <c r="R16" s="37">
         <f ca="1"/>
-        <v>0.14028896389690187</v>
+        <v>0.140197487625769</v>
       </c>
       <c r="S16" s="57">
         <f ca="1"/>
-        <v>-515039.82436631946</v>
+        <v>-527504.53199102578</v>
       </c>
       <c r="T16" s="57">
         <f ca="1"/>
-        <v>-10322.06696326</v>
+        <v>-22649.063679364997</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -7960,11 +7968,11 @@
       </c>
       <c r="F17" s="2">
         <f ca="1">F15+2</f>
-        <v>43206</v>
+        <v>43632</v>
       </c>
       <c r="G17" s="2">
         <f ca="1">F17+3</f>
-        <v>43209</v>
+        <v>43635</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>142</v>
@@ -8024,15 +8032,15 @@
       </c>
       <c r="R18" s="37">
         <f ca="1"/>
-        <v>-2.8896389690185529E-4</v>
+        <v>-1.97487625768998E-4</v>
       </c>
       <c r="S18" s="57">
         <f ca="1"/>
-        <v>618047.7892395833</v>
+        <v>633005.43838923087</v>
       </c>
       <c r="T18" s="57">
         <f ca="1"/>
-        <v>12386.480355911999</v>
+        <v>27178.876415238003</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -8053,11 +8061,11 @@
       </c>
       <c r="F19" s="2">
         <f ca="1">F17+2</f>
-        <v>43208</v>
+        <v>43634</v>
       </c>
       <c r="G19" s="2">
         <f ca="1">F19+3</f>
-        <v>43211</v>
+        <v>43637</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>142</v>
@@ -8120,15 +8128,15 @@
       </c>
       <c r="R20" s="37">
         <f ca="1"/>
-        <v>-2.8896389690185529E-4</v>
+        <v>-1.97487625768998E-4</v>
       </c>
       <c r="S20" s="57">
         <f ca="1"/>
-        <v>721055.75411284727</v>
+        <v>738506.34478743607</v>
       </c>
       <c r="T20" s="57">
         <f ca="1"/>
-        <v>14450.893748564</v>
+        <v>31708.689151111001</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -8149,11 +8157,11 @@
       </c>
       <c r="F21" s="2">
         <f ca="1">F19+2</f>
-        <v>43210</v>
+        <v>43636</v>
       </c>
       <c r="G21" s="2">
         <f ca="1">F21+3</f>
-        <v>43213</v>
+        <v>43639</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>142</v>
@@ -8215,15 +8223,15 @@
       </c>
       <c r="R22" s="37">
         <f ca="1"/>
-        <v>-2.8896389690185529E-4</v>
+        <v>-1.97487625768998E-4</v>
       </c>
       <c r="S22" s="57">
         <f ca="1"/>
-        <v>824063.71898611099</v>
+        <v>844007.25118564116</v>
       </c>
       <c r="T22" s="57">
         <f ca="1"/>
-        <v>16515.307141216002</v>
+        <v>36238.501886983999</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -8244,11 +8252,11 @@
       </c>
       <c r="F23" s="2">
         <f ca="1">F21+2</f>
-        <v>43212</v>
+        <v>43638</v>
       </c>
       <c r="G23" s="2">
         <f ca="1">F23+3</f>
-        <v>43215</v>
+        <v>43641</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>142</v>
@@ -8311,15 +8319,15 @@
       </c>
       <c r="R24" s="37">
         <f ca="1"/>
-        <v>0.14028896389690187</v>
+        <v>0.140197487625769</v>
       </c>
       <c r="S24" s="57">
         <f ca="1"/>
-        <v>-927071.68385937496</v>
+        <v>-949508.15758384624</v>
       </c>
       <c r="T24" s="57">
         <f ca="1"/>
-        <v>-18579.720533868</v>
+        <v>-40768.314622856997</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -8340,11 +8348,11 @@
       </c>
       <c r="F25" s="2">
         <f t="shared" ref="F25" ca="1" si="0">F23+2</f>
-        <v>43214</v>
+        <v>43640</v>
       </c>
       <c r="G25" s="2">
         <f ca="1">F25+3</f>
-        <v>43217</v>
+        <v>43643</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>142</v>
@@ -8399,15 +8407,15 @@
       </c>
       <c r="R26" s="37">
         <f ca="1"/>
-        <v>0.14028896389690187</v>
+        <v>0.140197487625769</v>
       </c>
       <c r="S26" s="57">
         <f ca="1"/>
-        <v>-1030079.6487326388</v>
+        <v>-1055009.0639820513</v>
       </c>
       <c r="T26" s="57">
         <f ca="1"/>
-        <v>-20644.13392652</v>
+        <v>-45298.127358729995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix to IB futures and some additional tests.
</commit_message>
<xml_diff>
--- a/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/BondTransactionPricer.xlsx
+++ b/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/BondTransactionPricer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2019\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Product Pricers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4114AEB-0FAC-4254-8214-513C5B8D05F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0274AB-6446-40F1-BA6A-A2D3EF553DE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="0" windowWidth="26370" windowHeight="14820" tabRatio="836" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="465" windowWidth="26370" windowHeight="14820" tabRatio="836" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AUDDiscountCurve" sheetId="10" r:id="rId1"/>
@@ -2191,7 +2191,7 @@
       <c r="F1" s="81"/>
       <c r="G1" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G2:H12, $C$18:$E$41)</f>
-        <v>Market.QR_LIVE.2019-06-25.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-08-18.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H1" s="122"/>
       <c r="I1" s="81"/>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="B3" s="85">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="C3" s="80"/>
       <c r="D3" s="80"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="H3" s="85">
         <f ca="1">H6</f>
-        <v>43641</v>
+        <v>43695</v>
       </c>
       <c r="I3" s="84"/>
     </row>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="B4" s="86">
         <f ca="1">B3</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="C4" s="80"/>
       <c r="D4" s="80"/>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="H4" s="86">
         <f ca="1">H3</f>
-        <v>43641</v>
+        <v>43695</v>
       </c>
       <c r="I4" s="84"/>
     </row>
@@ -2292,7 +2292,7 @@
       </c>
       <c r="H6" s="88">
         <f ca="1">'BondCurve-BondForward'!G7</f>
-        <v>43641</v>
+        <v>43695</v>
       </c>
       <c r="I6" s="84"/>
     </row>
@@ -2437,7 +2437,7 @@
       <c r="F14" s="84"/>
       <c r="G14" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G15:H25,HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-06-24.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-08-17.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H14" s="122"/>
       <c r="I14" s="84"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="H16" s="85">
         <f ca="1">H19</f>
-        <v>43640</v>
+        <v>43694</v>
       </c>
       <c r="I16" s="84"/>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="H17" s="86">
         <f ca="1">H16</f>
-        <v>43640</v>
+        <v>43694</v>
       </c>
       <c r="I17" s="84"/>
     </row>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="H19" s="88">
         <f ca="1">'BondCurve-BondForward'!G21</f>
-        <v>43640</v>
+        <v>43694</v>
       </c>
       <c r="I19" s="84"/>
     </row>
@@ -2752,7 +2752,7 @@
       <c r="F27" s="84"/>
       <c r="G27" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G28:H38, HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-06-23.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-08-16.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H27" s="122"/>
       <c r="I27" s="84"/>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="H29" s="85">
         <f ca="1">H32</f>
-        <v>43639</v>
+        <v>43693</v>
       </c>
       <c r="I29" s="84"/>
     </row>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="H30" s="86">
         <f ca="1">H29</f>
-        <v>43639</v>
+        <v>43693</v>
       </c>
       <c r="I30" s="84"/>
     </row>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="H32" s="88">
         <f ca="1">'BondCurve-BondForward'!G35</f>
-        <v>43639</v>
+        <v>43693</v>
       </c>
       <c r="I32" s="84"/>
     </row>
@@ -3088,7 +3088,7 @@
       <c r="F40" s="84"/>
       <c r="G40" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G41:H51, HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-06-22.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-08-15.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H40" s="122"/>
       <c r="I40" s="84"/>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="H42" s="85">
         <f ca="1">H45</f>
-        <v>43638</v>
+        <v>43692</v>
       </c>
       <c r="I42" s="84"/>
     </row>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="H43" s="86">
         <f ca="1">H42</f>
-        <v>43638</v>
+        <v>43692</v>
       </c>
       <c r="I43" s="84"/>
     </row>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="H45" s="88">
         <f ca="1">'BondCurve-BondForward'!G49</f>
-        <v>43638</v>
+        <v>43692</v>
       </c>
       <c r="I45" s="82"/>
     </row>
@@ -3237,7 +3237,7 @@
     <row r="53" spans="7:8" ht="13.5" thickBot="1">
       <c r="G53" s="121" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G54:H64, HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-06-21.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-08-14.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H53" s="122"/>
     </row>
@@ -3255,7 +3255,7 @@
       </c>
       <c r="H55" s="85">
         <f ca="1">H58</f>
-        <v>43637</v>
+        <v>43691</v>
       </c>
     </row>
     <row r="56" spans="7:8">
@@ -3264,7 +3264,7 @@
       </c>
       <c r="H56" s="86">
         <f ca="1">H55</f>
-        <v>43637</v>
+        <v>43691</v>
       </c>
     </row>
     <row r="57" spans="7:8">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H58" s="88">
         <f ca="1">'BondCurve-BondForward'!G63</f>
-        <v>43637</v>
+        <v>43691</v>
       </c>
     </row>
     <row r="59" spans="7:8">
@@ -3406,7 +3406,7 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C39" s="31">
         <f ca="1"/>
-        <v>2.5000000000000012E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="40" spans="2:3">
@@ -3698,7 +3698,7 @@
       </c>
       <c r="C40" s="31">
         <f ca="1"/>
-        <v>2.5000000000000012E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="2:3">
@@ -3778,7 +3778,7 @@
       <c r="C2" s="124"/>
       <c r="F2" s="123" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F3:G15, $B$18:$D$21)</f>
-        <v>Market.QR_LIVE.2019-06-25.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-08-18.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G2" s="124"/>
     </row>
@@ -3802,14 +3802,14 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="25">
         <f ca="1">G7</f>
-        <v>43641</v>
+        <v>43695</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -3818,14 +3818,14 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="26">
         <f ca="1">G4</f>
-        <v>43641</v>
+        <v>43695</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -3843,7 +3843,7 @@
       </c>
       <c r="I6" t="str">
         <f ca="1">G6&amp;"."&amp;TEXT(G7,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-06-25</v>
+        <v>QR_LIVE.2019-08-18</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -3858,11 +3858,11 @@
       </c>
       <c r="G7" s="77">
         <f ca="1">$C$5-1</f>
-        <v>43641</v>
+        <v>43695</v>
       </c>
       <c r="I7" t="str">
         <f ca="1">G20&amp;"."&amp;TEXT(G21,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-06-24</v>
+        <v>QR_LIVE.2019-08-17</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -3880,7 +3880,7 @@
       </c>
       <c r="I8" t="str">
         <f ca="1">G34&amp;"."&amp;TEXT(G35,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-06-23</v>
+        <v>QR_LIVE.2019-08-16</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="I9" t="str">
         <f ca="1">G48&amp;"."&amp;TEXT(G49,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-06-22</v>
+        <v>QR_LIVE.2019-08-15</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -3916,7 +3916,7 @@
       </c>
       <c r="I10" t="str">
         <f ca="1">G62&amp;"."&amp;TEXT(G63,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-06-21</v>
+        <v>QR_LIVE.2019-08-14</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -3989,7 +3989,7 @@
       <c r="D16" s="13"/>
       <c r="F16" s="125" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F17:G29, $B$23:$D$26)</f>
-        <v>Market.QR_LIVE.2019-06-24.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-08-17.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G16" s="126"/>
     </row>
@@ -4025,7 +4025,7 @@
       </c>
       <c r="G18" s="25">
         <f ca="1">G21</f>
-        <v>43640</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="19" spans="2:7">
@@ -4043,7 +4043,7 @@
       </c>
       <c r="G19" s="26">
         <f ca="1">G18</f>
-        <v>43640</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="20" spans="2:7">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="G21" s="77">
         <f ca="1">$G$7-1</f>
-        <v>43640</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="13.5" thickBot="1">
@@ -4212,7 +4212,7 @@
       </c>
       <c r="F30" s="125" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F31:G43, $B$28:$D$31)</f>
-        <v>Market.QR_LIVE.2019-06-23.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-08-16.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G30" s="126"/>
     </row>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="G32" s="25">
         <f ca="1">G35</f>
-        <v>43639</v>
+        <v>43693</v>
       </c>
     </row>
     <row r="33" spans="2:7">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="G33" s="26">
         <f ca="1">G32</f>
-        <v>43639</v>
+        <v>43693</v>
       </c>
     </row>
     <row r="34" spans="2:7">
@@ -4293,7 +4293,7 @@
       </c>
       <c r="G35" s="77">
         <f ca="1">$G$7-2</f>
-        <v>43639</v>
+        <v>43693</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="13.5" thickBot="1">
@@ -4411,7 +4411,7 @@
       </c>
       <c r="F44" s="125" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F45:G57, $B$33:$D$36)</f>
-        <v>Market.QR_LIVE.2019-06-22.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-08-15.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G44" s="126"/>
     </row>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="G46" s="25">
         <f ca="1">G49</f>
-        <v>43638</v>
+        <v>43692</v>
       </c>
     </row>
     <row r="47" spans="2:7">
@@ -4462,7 +4462,7 @@
       </c>
       <c r="G47" s="26">
         <f ca="1">G46</f>
-        <v>43638</v>
+        <v>43692</v>
       </c>
     </row>
     <row r="48" spans="2:7">
@@ -4496,7 +4496,7 @@
       </c>
       <c r="G49" s="77">
         <f ca="1">$G$7-3</f>
-        <v>43638</v>
+        <v>43692</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="13.5" thickBot="1">
@@ -4521,7 +4521,7 @@
     <row r="52" spans="2:7">
       <c r="B52" s="73">
         <f t="array" aca="1" ref="B52:C56" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="C52" s="30">
         <f ca="1"/>
@@ -4537,7 +4537,7 @@
     <row r="53" spans="2:7">
       <c r="B53" s="74">
         <f ca="1"/>
-        <v>43644</v>
+        <v>43698</v>
       </c>
       <c r="C53" s="31">
         <f ca="1"/>
@@ -4553,7 +4553,7 @@
     <row r="54" spans="2:7">
       <c r="B54" s="74">
         <f ca="1"/>
-        <v>43675</v>
+        <v>43731</v>
       </c>
       <c r="C54" s="31">
         <f ca="1"/>
@@ -4569,7 +4569,7 @@
     <row r="55" spans="2:7">
       <c r="B55" s="74">
         <f ca="1"/>
-        <v>43705</v>
+        <v>43759</v>
       </c>
       <c r="C55" s="31">
         <f ca="1"/>
@@ -4612,14 +4612,14 @@
       </c>
       <c r="F58" s="125" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F59:G71, $B$38:$D$41)</f>
-        <v>Market.QR_LIVE.2019-06-21.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-08-14.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G58" s="126"/>
     </row>
     <row r="59" spans="2:7" ht="13.5" thickBot="1">
       <c r="B59" s="73">
         <f ca="1">B52</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="C59" s="30">
         <f t="array" aca="1" ref="C59:C63" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B52:B56)</f>
@@ -4635,7 +4635,7 @@
     <row r="60" spans="2:7">
       <c r="B60" s="74">
         <f t="shared" ref="B60:B63" ca="1" si="0">B53</f>
-        <v>43644</v>
+        <v>43698</v>
       </c>
       <c r="C60" s="31">
         <f ca="1"/>
@@ -4646,13 +4646,13 @@
       </c>
       <c r="G60" s="25">
         <f ca="1">G63</f>
-        <v>43637</v>
+        <v>43691</v>
       </c>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43675</v>
+        <v>43731</v>
       </c>
       <c r="C61" s="31">
         <f ca="1"/>
@@ -4663,13 +4663,13 @@
       </c>
       <c r="G61" s="26">
         <f ca="1">G60</f>
-        <v>43637</v>
+        <v>43691</v>
       </c>
     </row>
     <row r="62" spans="2:7">
       <c r="B62" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43705</v>
+        <v>43759</v>
       </c>
       <c r="C62" s="31">
         <f ca="1"/>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="G63" s="77">
         <f ca="1">$G$7-4</f>
-        <v>43637</v>
+        <v>43691</v>
       </c>
     </row>
     <row r="64" spans="2:7">
@@ -4815,7 +4815,7 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -4824,7 +4824,7 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -5032,7 +5032,7 @@
     <row r="32" spans="2:4">
       <c r="B32" s="73">
         <f t="array" aca="1" ref="B32:C36" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="C32" s="30">
         <f ca="1"/>
@@ -5042,7 +5042,7 @@
     <row r="33" spans="2:3">
       <c r="B33" s="74">
         <f ca="1"/>
-        <v>43643</v>
+        <v>43697</v>
       </c>
       <c r="C33" s="31">
         <f ca="1"/>
@@ -5052,27 +5052,27 @@
     <row r="34" spans="2:3">
       <c r="B34" s="74">
         <f ca="1"/>
-        <v>43675</v>
+        <v>43728</v>
       </c>
       <c r="C34" s="31">
         <f ca="1"/>
-        <v>0.99549920035018302</v>
+        <v>0.99563499344803497</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="74">
         <f ca="1"/>
-        <v>43704</v>
+        <v>43759</v>
       </c>
       <c r="C35" s="31">
         <f ca="1"/>
-        <v>0.99157724996162799</v>
+        <v>0.99144256139195097</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="13.5" thickBot="1">
       <c r="B36" s="75">
         <f ca="1"/>
-        <v>43735</v>
+        <v>43789</v>
       </c>
       <c r="C36" s="32">
         <f ca="1"/>
@@ -5088,7 +5088,7 @@
     <row r="39" spans="2:3">
       <c r="B39" s="73">
         <f ca="1">B32</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="C39" s="30">
         <f t="array" aca="1" ref="C39:C43" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B32:B36)</f>
@@ -5098,7 +5098,7 @@
     <row r="40" spans="2:3">
       <c r="B40" s="74">
         <f t="shared" ref="B40:B43" ca="1" si="0">B33</f>
-        <v>43643</v>
+        <v>43697</v>
       </c>
       <c r="C40" s="31">
         <f ca="1"/>
@@ -5108,27 +5108,27 @@
     <row r="41" spans="2:3">
       <c r="B41" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43675</v>
+        <v>43728</v>
       </c>
       <c r="C41" s="31">
         <f ca="1"/>
-        <v>0.99549920035018302</v>
+        <v>0.99563499344803497</v>
       </c>
     </row>
     <row r="42" spans="2:3">
       <c r="B42" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43704</v>
+        <v>43759</v>
       </c>
       <c r="C42" s="31">
         <f ca="1"/>
-        <v>0.99157724996162799</v>
+        <v>0.99144256139195097</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="13.5" thickBot="1">
       <c r="B43" s="75">
         <f t="shared" ca="1" si="0"/>
-        <v>43735</v>
+        <v>43789</v>
       </c>
       <c r="C43" s="32">
         <f ca="1"/>
@@ -5220,14 +5220,14 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="25">
         <f ca="1">G5</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -5236,14 +5236,14 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -5451,7 +5451,7 @@
       </c>
       <c r="G20" s="25">
         <f ca="1">G21</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="G21" s="26">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="22" spans="2:7">
@@ -5571,7 +5571,7 @@
       </c>
       <c r="C28" s="65">
         <f ca="1"/>
-        <v>5.0006635273972595E-2</v>
+        <v>5.000658682216922E-2</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>35</v>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="C29" s="65">
         <f ca="1"/>
-        <v>5.0006741489319828E-2</v>
+        <v>5.0006738842245456E-2</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>37</v>
@@ -5603,7 +5603,7 @@
       </c>
       <c r="C30" s="65">
         <f ca="1"/>
-        <v>5.0006799734284978E-2</v>
+        <v>5.0006783133467556E-2</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>38</v>
@@ -5650,7 +5650,7 @@
     <row r="34" spans="2:7" ht="13.5" thickBot="1">
       <c r="B34" s="73">
         <f t="array" aca="1" ref="B34:C38" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="C34" s="64">
         <f ca="1"/>
@@ -5665,7 +5665,7 @@
     <row r="35" spans="2:7" ht="13.5" thickBot="1">
       <c r="B35" s="74">
         <f ca="1"/>
-        <v>43643</v>
+        <v>43697</v>
       </c>
       <c r="C35" s="65">
         <f ca="1"/>
@@ -5681,45 +5681,45 @@
     <row r="36" spans="2:7">
       <c r="B36" s="74">
         <f ca="1"/>
-        <v>43675</v>
+        <v>43728</v>
       </c>
       <c r="C36" s="65">
         <f ca="1"/>
-        <v>0.99549862334982497</v>
+        <v>0.99563443844231203</v>
       </c>
       <c r="F36" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G36" s="25">
         <f ca="1">G37</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="74">
         <f ca="1"/>
-        <v>43704</v>
+        <v>43759</v>
       </c>
       <c r="C37" s="65">
         <f ca="1"/>
-        <v>0.99157614205086997</v>
+        <v>0.99144143606670698</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G37" s="26">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="13.5" thickBot="1">
       <c r="B38" s="75">
         <f ca="1"/>
-        <v>43735</v>
+        <v>43789</v>
       </c>
       <c r="C38" s="66">
         <f ca="1"/>
-        <v>0.98741717842536103</v>
+        <v>0.98741718250559696</v>
       </c>
       <c r="F38" s="22" t="s">
         <v>26</v>
@@ -5752,7 +5752,7 @@
     <row r="41" spans="2:7">
       <c r="B41" s="73">
         <f ca="1">B34</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="C41" s="64">
         <f t="array" aca="1" ref="C41:C45" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B34:B38)</f>
@@ -5768,7 +5768,7 @@
     <row r="42" spans="2:7">
       <c r="B42" s="74">
         <f t="shared" ref="B42:B45" ca="1" si="0">B35</f>
-        <v>43643</v>
+        <v>43697</v>
       </c>
       <c r="C42" s="65">
         <f ca="1"/>
@@ -5784,11 +5784,11 @@
     <row r="43" spans="2:7">
       <c r="B43" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43675</v>
+        <v>43728</v>
       </c>
       <c r="C43" s="65">
         <f ca="1"/>
-        <v>5.0212902395297299E-2</v>
+        <v>5.0216290738325703E-2</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>34</v>
@@ -5800,11 +5800,11 @@
     <row r="44" spans="2:7">
       <c r="B44" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43704</v>
+        <v>43759</v>
       </c>
       <c r="C44" s="65">
         <f ca="1"/>
-        <v>5.0113447890619299E-2</v>
+        <v>5.0110018589199598E-2</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>35</v>
@@ -5816,11 +5816,11 @@
     <row r="45" spans="2:7" ht="13.5" thickBot="1">
       <c r="B45" s="75">
         <f t="shared" ca="1" si="0"/>
-        <v>43735</v>
+        <v>43789</v>
       </c>
       <c r="C45" s="66">
         <f ca="1"/>
-        <v>5.0007532584952899E-2</v>
+        <v>5.0007516164302303E-2</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>37</v>
@@ -5892,7 +5892,7 @@
       </c>
       <c r="G52" s="25">
         <f ca="1">G53</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="53" spans="2:7">
@@ -5901,7 +5901,7 @@
       </c>
       <c r="G53" s="26">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
     </row>
     <row r="54" spans="2:7">
@@ -6017,10 +6017,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:G45"/>
+  <dimension ref="B1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6029,23 +6029,40 @@
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" customWidth="1"/>
-    <col min="5" max="5" width="86.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7">
-      <c r="G1" t="str">
-        <f t="array" ref="G1:G13">_xll.HLV5r3.Financial.Cache.SupportedBondMetrics()</f>
+    <row r="1" spans="2:9">
+      <c r="F1" t="str">
+        <f t="array" ref="F1:F13">_xll.HLV5r3.Financial.Cache.SupportedBondMetrics()</f>
         <v>DirtyPrice</v>
       </c>
-    </row>
-    <row r="2" spans="2:7">
-      <c r="G2" t="str">
+      <c r="H1" s="1" t="e">
+        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I1,$C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I1" t="str">
+        <f>'BondCurve-BondForward'!C6</f>
+        <v>QR_LIVE</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
+      <c r="F2" t="str">
         <v>CleanPrice</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
+      <c r="H2" s="1" t="e">
+        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I2,$C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I2" t="str">
+        <f ca="1">'BondCurve-BondForward'!I6</f>
+        <v>QR_LIVE.2019-08-18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -6055,11 +6072,19 @@
       <c r="E3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="str">
+      <c r="F3" t="str">
         <v>NPV</v>
       </c>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="H3" s="1" t="e">
+        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I3,$C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I3" t="str">
+        <f ca="1">'BondCurve-BondForward'!I7</f>
+        <v>QR_LIVE.2019-08-17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -6069,11 +6094,19 @@
       <c r="E4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="str">
+      <c r="F4" t="str">
         <v>AccruedInterest</v>
       </c>
-    </row>
-    <row r="5" spans="2:7">
+      <c r="H4" s="1" t="e">
+        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I4,$C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I4" t="str">
+        <f ca="1">'BondCurve-BondForward'!I8</f>
+        <v>QR_LIVE.2019-08-16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -6083,11 +6116,19 @@
       <c r="E5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G5" t="str">
+      <c r="F5" t="str">
         <v>ImpliedQuote</v>
       </c>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="H5" s="1" t="e">
+        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I5,$C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I5" t="str">
+        <f ca="1">'BondCurve-BondForward'!I9</f>
+        <v>QR_LIVE.2019-08-15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -6097,76 +6138,84 @@
       <c r="E6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G6" t="str">
+      <c r="F6" t="str">
         <v>Convexity</v>
       </c>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="H6" s="1" t="e">
+        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I6,$C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I6" t="str">
+        <f ca="1">'BondCurve-BondForward'!I10</f>
+        <v>QR_LIVE.2019-08-14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
       <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G7" t="str">
+      <c r="F7" t="str">
         <v>DeltaR</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>141</v>
       </c>
       <c r="C8" t="s">
         <v>142</v>
       </c>
-      <c r="G8" t="str">
+      <c r="F8" t="str">
         <v>DV01</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="3">
         <v>100000000</v>
       </c>
-      <c r="G9" t="str">
+      <c r="F9" t="str">
         <v>MarketQuote</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
-      </c>
-      <c r="G10" t="str">
+        <v>43696</v>
+      </c>
+      <c r="F10" t="str">
         <v>AssetSwapSpread</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="2">
         <f ca="1">C10+5</f>
-        <v>43647</v>
-      </c>
-      <c r="G11" t="str">
+        <v>43701</v>
+      </c>
+      <c r="F11" t="str">
         <v>ZSpread</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:9">
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
       </c>
-      <c r="G12" t="str">
+      <c r="F12" t="str">
         <v>YieldToMaturity</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -6176,22 +6225,22 @@
       <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="G13" t="str">
+      <c r="F13" t="str">
         <v>PandL</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:9">
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
         <v>144</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:9">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -6199,21 +6248,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:9">
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="2">
         <f ca="1">C10</f>
-        <v>43642</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="array" aca="1" ref="E16:F22" ca="1">_xll.HLV5r3.Financial.Cache.ViewValuationReport(E28)</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="F16" s="60">
-        <f ca="1"/>
-        <v>0.05</v>
+        <v>43696</v>
+      </c>
+      <c r="E16" t="e">
+        <f t="array" aca="1" ref="E16:F22" ca="1">_xll.HLV5r3.Financial.Cache.ViewValuationReport(H1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F16" s="60" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -6223,13 +6272,13 @@
       <c r="C17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E17" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="F17" s="60">
-        <f ca="1"/>
-        <v>-1.97487625768998E-4</v>
+      <c r="E17" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F17" s="60" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -6239,13 +6288,13 @@
       <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="F18" s="115">
-        <f ca="1"/>
-        <v>105500906.39820515</v>
+      <c r="E18" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="115" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -6255,13 +6304,13 @@
       <c r="C19" t="s">
         <v>1</v>
       </c>
-      <c r="E19" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
-      </c>
-      <c r="F19" s="115">
-        <f ca="1"/>
-        <v>4529812.7358730007</v>
+      <c r="E19" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="115" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="2:6">
@@ -6271,13 +6320,13 @@
       <c r="C20" t="s">
         <v>49</v>
       </c>
-      <c r="E20" t="str">
-        <f ca="1"/>
-        <v>DirtyPrice</v>
-      </c>
-      <c r="F20">
-        <f ca="1"/>
-        <v>1.0552981273587301</v>
+      <c r="E20" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F20" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="2:6">
@@ -6289,11 +6338,11 @@
       </c>
       <c r="E21" t="e">
         <f ca="1"/>
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F21" t="e">
         <f ca="1"/>
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="2:6">
@@ -6304,11 +6353,11 @@
       <c r="C22" s="127"/>
       <c r="E22" t="e">
         <f ca="1"/>
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F22" t="e">
         <f ca="1"/>
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="2:6">
@@ -6320,6 +6369,10 @@
         <f ca="1"/>
         <v>Party1</v>
       </c>
+      <c r="E24" t="e">
+        <f t="array" aca="1" ref="E24" ca="1">_xll.HLV5r3.Financial.Cache.ViewExpectedCashFlows(B22,C18,E3:E7,C27,$I$1,C16)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" t="str">
@@ -6360,14 +6413,6 @@
         <f ca="1"/>
         <v>43753</v>
       </c>
-      <c r="E28" s="1" t="str">
-        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F28,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE</v>
-      </c>
-      <c r="F28" t="str">
-        <f>'BondCurve-BondForward'!C6</f>
-        <v>QR_LIVE</v>
-      </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" t="str">
@@ -6378,14 +6423,6 @@
         <f ca="1"/>
         <v>Fixed</v>
       </c>
-      <c r="E29" s="1" t="str">
-        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F29,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-25</v>
-      </c>
-      <c r="F29" t="str">
-        <f ca="1">'BondCurve-BondForward'!I6</f>
-        <v>QR_LIVE.2019-06-25</v>
-      </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" t="str">
@@ -6396,14 +6433,6 @@
         <f ca="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E30" s="1" t="str">
-        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F30,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-24</v>
-      </c>
-      <c r="F30" t="str">
-        <f ca="1">'BondCurve-BondForward'!I7</f>
-        <v>QR_LIVE.2019-06-24</v>
-      </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" t="str">
@@ -6414,14 +6443,6 @@
         <f ca="1"/>
         <v>ACT/ACT.ISDA</v>
       </c>
-      <c r="E31" s="1" t="str">
-        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F31,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-23</v>
-      </c>
-      <c r="F31" t="str">
-        <f ca="1">'BondCurve-BondForward'!I8</f>
-        <v>QR_LIVE.2019-06-23</v>
-      </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" t="str">
@@ -6432,16 +6453,8 @@
         <f ca="1"/>
         <v>6M</v>
       </c>
-      <c r="E32" s="1" t="str">
-        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F32,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-22</v>
-      </c>
-      <c r="F32" t="str">
-        <f ca="1">'BondCurve-BondForward'!I9</f>
-        <v>QR_LIVE.2019-06-22</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
+    </row>
+    <row r="33" spans="2:3">
       <c r="B33" t="str">
         <f ca="1"/>
         <v>party1</v>
@@ -6450,16 +6463,8 @@
         <f ca="1"/>
         <v>CBA</v>
       </c>
-      <c r="E33" s="1" t="str">
-        <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",F33,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-06-21</v>
-      </c>
-      <c r="F33" t="str">
-        <f ca="1">'BondCurve-BondForward'!I10</f>
-        <v>QR_LIVE.2019-06-21</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
+    </row>
+    <row r="34" spans="2:3">
       <c r="B34" t="str">
         <f ca="1"/>
         <v>party2</v>
@@ -6469,7 +6474,7 @@
         <v>NAB</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:3">
       <c r="B35" t="str">
         <f ca="1"/>
         <v>description</v>
@@ -6479,7 +6484,7 @@
         <v>WATC 7 10/15/19</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:3">
       <c r="B36" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6489,7 +6494,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:3">
       <c r="B37" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6499,7 +6504,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:3">
       <c r="B38" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6509,7 +6514,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:3">
       <c r="B39" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6519,7 +6524,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:3">
       <c r="B40" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6529,7 +6534,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:3">
       <c r="B41" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6539,7 +6544,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:3">
       <c r="B42" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6549,7 +6554,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:3">
       <c r="B43" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6559,7 +6564,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:3">
       <c r="B44" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6569,7 +6574,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="2:6">
+    <row r="45" spans="2:3">
       <c r="B45" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6592,7 +6597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
@@ -6717,7 +6722,7 @@
       </c>
       <c r="C10" s="2">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="E10" s="114" t="s">
         <v>140</v>
@@ -6735,7 +6740,7 @@
       </c>
       <c r="C11" s="2">
         <f ca="1">C10+5</f>
-        <v>43647</v>
+        <v>43701</v>
       </c>
       <c r="H11" t="str">
         <v>ZSpread</v>
@@ -6791,7 +6796,7 @@
       </c>
       <c r="C16" s="2">
         <f ca="1">C10</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="E16" s="61" t="str">
         <f t="array" ref="E16:F22">_xll.HLV5r3.Financial.Cache.ViewValuationReport(E27)</f>
@@ -6959,13 +6964,13 @@
         <f ca="1"/>
         <v>Fixed</v>
       </c>
-      <c r="E29" s="1" t="str">
+      <c r="E29" s="1" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarkets($C$22,$E$24,$C$18,$E$3:$E$7,"AUD",$H$29:$H$33,$C$10)</f>
-        <v>Var_Run_20170531</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H29" s="1" t="str">
         <f t="array" aca="1" ref="H29:H33" ca="1">Markets</f>
-        <v>QR_LIVE.2019-06-25</v>
+        <v>QR_LIVE.2019-08-18</v>
       </c>
     </row>
     <row r="30" spans="2:8">
@@ -6979,7 +6984,7 @@
       </c>
       <c r="H30" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-06-24</v>
+        <v>QR_LIVE.2019-08-17</v>
       </c>
     </row>
     <row r="31" spans="2:8">
@@ -6993,7 +6998,7 @@
       </c>
       <c r="H31" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-06-23</v>
+        <v>QR_LIVE.2019-08-16</v>
       </c>
     </row>
     <row r="32" spans="2:8">
@@ -7014,7 +7019,7 @@
       </c>
       <c r="H32" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-06-22</v>
+        <v>QR_LIVE.2019-08-15</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -7034,7 +7039,7 @@
       </c>
       <c r="H33" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-06-21</v>
+        <v>QR_LIVE.2019-08-14</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -7388,7 +7393,7 @@
       </c>
       <c r="K3" s="50">
         <f ca="1">TODAY()</f>
-        <v>43642</v>
+        <v>43696</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>21</v>
@@ -7497,11 +7502,11 @@
       </c>
       <c r="F7" s="2">
         <f ca="1">TODAY()-20</f>
-        <v>43622</v>
+        <v>43676</v>
       </c>
       <c r="G7" s="2">
         <f ca="1">F7+3</f>
-        <v>43625</v>
+        <v>43679</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>142</v>
@@ -7528,43 +7533,43 @@
       <c r="O7">
         <v>101</v>
       </c>
-      <c r="P7" t="str">
+      <c r="P7" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K7,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.001.QR_LIVE</v>
-      </c>
-      <c r="Q7" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q7" t="e">
         <f t="array" aca="1" ref="Q7:T8" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P7))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R7" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S7" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T7" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R7" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S7" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T7" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="Q8" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R8" s="37">
-        <f ca="1"/>
-        <v>-1.97487625768998E-4</v>
-      </c>
-      <c r="S8" s="57">
-        <f ca="1"/>
-        <v>105500.90639820514</v>
-      </c>
-      <c r="T8" s="57">
-        <f ca="1"/>
-        <v>4529.8127358729998</v>
+      <c r="Q8" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R8" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S8" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T8" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -7585,11 +7590,11 @@
       </c>
       <c r="F9" s="2">
         <f ca="1">F7+2</f>
-        <v>43624</v>
+        <v>43678</v>
       </c>
       <c r="G9" s="2">
         <f ca="1">F9+3</f>
-        <v>43627</v>
+        <v>43681</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>142</v>
@@ -7616,25 +7621,25 @@
       <c r="O9">
         <v>101</v>
       </c>
-      <c r="P9" t="str">
+      <c r="P9" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K9,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.002.QR_LIVE</v>
-      </c>
-      <c r="Q9" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q9" t="e">
         <f t="array" aca="1" ref="Q9:T10" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P9))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R9" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S9" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T9" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R9" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S9" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T9" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -7646,21 +7651,21 @@
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
       <c r="N10" s="7"/>
-      <c r="Q10" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R10" s="37">
-        <f ca="1"/>
-        <v>-1.97487625768998E-4</v>
-      </c>
-      <c r="S10" s="57">
-        <f ca="1"/>
-        <v>211001.81279641029</v>
-      </c>
-      <c r="T10" s="57">
-        <f ca="1"/>
-        <v>9059.6254717459997</v>
+      <c r="Q10" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R10" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S10" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T10" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -7681,11 +7686,11 @@
       </c>
       <c r="F11" s="2">
         <f ca="1">F9+2</f>
-        <v>43626</v>
+        <v>43680</v>
       </c>
       <c r="G11" s="2">
         <f ca="1">F11+3</f>
-        <v>43629</v>
+        <v>43683</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>142</v>
@@ -7712,25 +7717,25 @@
       <c r="O11">
         <v>101</v>
       </c>
-      <c r="P11" t="str">
+      <c r="P11" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K11,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.003.QR_LIVE</v>
-      </c>
-      <c r="Q11" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q11" t="e">
         <f t="array" aca="1" ref="Q11:T12" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P11))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R11" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S11" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T11" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R11" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S11" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T11" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -7742,21 +7747,21 @@
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
       <c r="N12" s="7"/>
-      <c r="Q12" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R12" s="37">
-        <f ca="1"/>
-        <v>-1.97487625768998E-4</v>
-      </c>
-      <c r="S12" s="57">
-        <f ca="1"/>
-        <v>316502.71919461543</v>
-      </c>
-      <c r="T12" s="57">
-        <f ca="1"/>
-        <v>13589.438207619001</v>
+      <c r="Q12" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R12" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S12" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T12" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -7777,11 +7782,11 @@
       </c>
       <c r="F13" s="2">
         <f ca="1">F11+2</f>
-        <v>43628</v>
+        <v>43682</v>
       </c>
       <c r="G13" s="2">
         <f ca="1">F13+3</f>
-        <v>43631</v>
+        <v>43685</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>142</v>
@@ -7808,25 +7813,25 @@
       <c r="O13">
         <v>101</v>
       </c>
-      <c r="P13" t="str">
+      <c r="P13" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K13,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.004.QR_LIVE</v>
-      </c>
-      <c r="Q13" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q13" t="e">
         <f t="array" aca="1" ref="Q13:T14" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P13))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R13" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S13" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T13" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S13" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T13" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -7838,21 +7843,21 @@
       <c r="H14" s="2"/>
       <c r="I14" s="3"/>
       <c r="N14" s="7"/>
-      <c r="Q14" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R14" s="37">
-        <f ca="1"/>
-        <v>0.140197487625769</v>
-      </c>
-      <c r="S14" s="57">
-        <f ca="1"/>
-        <v>-422003.62559282058</v>
-      </c>
-      <c r="T14" s="57">
-        <f ca="1"/>
-        <v>-18119.250943491999</v>
+      <c r="Q14" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R14" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S14" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T14" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -7873,11 +7878,11 @@
       </c>
       <c r="F15" s="2">
         <f ca="1">F13+2</f>
-        <v>43630</v>
+        <v>43684</v>
       </c>
       <c r="G15" s="2">
         <f ca="1">F15+3</f>
-        <v>43633</v>
+        <v>43687</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>142</v>
@@ -7904,25 +7909,25 @@
       <c r="O15">
         <v>101</v>
       </c>
-      <c r="P15" t="str">
+      <c r="P15" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K15,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.005.QR_LIVE</v>
-      </c>
-      <c r="Q15" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q15" t="e">
         <f t="array" aca="1" ref="Q15:T16" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P15))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R15" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S15" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T15" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R15" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S15" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T15" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -7933,21 +7938,21 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
-      <c r="Q16" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R16" s="37">
-        <f ca="1"/>
-        <v>0.140197487625769</v>
-      </c>
-      <c r="S16" s="57">
-        <f ca="1"/>
-        <v>-527504.53199102578</v>
-      </c>
-      <c r="T16" s="57">
-        <f ca="1"/>
-        <v>-22649.063679364997</v>
+      <c r="Q16" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R16" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S16" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T16" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -7968,11 +7973,11 @@
       </c>
       <c r="F17" s="2">
         <f ca="1">F15+2</f>
-        <v>43632</v>
+        <v>43686</v>
       </c>
       <c r="G17" s="2">
         <f ca="1">F17+3</f>
-        <v>43635</v>
+        <v>43689</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>142</v>
@@ -7999,25 +8004,25 @@
       <c r="O17">
         <v>101</v>
       </c>
-      <c r="P17" t="str">
+      <c r="P17" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K17,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.006.QR_LIVE</v>
-      </c>
-      <c r="Q17" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q17" t="e">
         <f t="array" aca="1" ref="Q17:T18" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P17))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R17" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S17" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T17" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R17" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S17" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T17" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -8026,21 +8031,21 @@
       <c r="G18" s="2"/>
       <c r="I18" s="3"/>
       <c r="N18" s="7"/>
-      <c r="Q18" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R18" s="37">
-        <f ca="1"/>
-        <v>-1.97487625768998E-4</v>
-      </c>
-      <c r="S18" s="57">
-        <f ca="1"/>
-        <v>633005.43838923087</v>
-      </c>
-      <c r="T18" s="57">
-        <f ca="1"/>
-        <v>27178.876415238003</v>
+      <c r="Q18" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R18" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S18" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T18" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -8061,11 +8066,11 @@
       </c>
       <c r="F19" s="2">
         <f ca="1">F17+2</f>
-        <v>43634</v>
+        <v>43688</v>
       </c>
       <c r="G19" s="2">
         <f ca="1">F19+3</f>
-        <v>43637</v>
+        <v>43691</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>142</v>
@@ -8092,25 +8097,25 @@
       <c r="O19">
         <v>101</v>
       </c>
-      <c r="P19" t="str">
+      <c r="P19" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K19,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.007.QR_LIVE</v>
-      </c>
-      <c r="Q19" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q19" t="e">
         <f t="array" aca="1" ref="Q19:T20" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P19))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R19" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S19" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T19" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R19" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S19" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T19" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -8122,21 +8127,21 @@
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
       <c r="N20" s="7"/>
-      <c r="Q20" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R20" s="37">
-        <f ca="1"/>
-        <v>-1.97487625768998E-4</v>
-      </c>
-      <c r="S20" s="57">
-        <f ca="1"/>
-        <v>738506.34478743607</v>
-      </c>
-      <c r="T20" s="57">
-        <f ca="1"/>
-        <v>31708.689151111001</v>
+      <c r="Q20" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R20" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S20" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T20" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -8157,11 +8162,11 @@
       </c>
       <c r="F21" s="2">
         <f ca="1">F19+2</f>
-        <v>43636</v>
+        <v>43690</v>
       </c>
       <c r="G21" s="2">
         <f ca="1">F21+3</f>
-        <v>43639</v>
+        <v>43693</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>142</v>
@@ -8188,25 +8193,25 @@
       <c r="O21">
         <v>101</v>
       </c>
-      <c r="P21" t="str">
+      <c r="P21" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K21,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.008.QR_LIVE</v>
-      </c>
-      <c r="Q21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q21" t="e">
         <f t="array" aca="1" ref="Q21:T22" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P21))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R21" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S21" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T21" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R21" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S21" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T21" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -8217,21 +8222,21 @@
       <c r="H22" s="2"/>
       <c r="I22" s="3"/>
       <c r="N22" s="7"/>
-      <c r="Q22" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R22" s="37">
-        <f ca="1"/>
-        <v>-1.97487625768998E-4</v>
-      </c>
-      <c r="S22" s="57">
-        <f ca="1"/>
-        <v>844007.25118564116</v>
-      </c>
-      <c r="T22" s="57">
-        <f ca="1"/>
-        <v>36238.501886983999</v>
+      <c r="Q22" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R22" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S22" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T22" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -8252,11 +8257,11 @@
       </c>
       <c r="F23" s="2">
         <f ca="1">F21+2</f>
-        <v>43638</v>
+        <v>43692</v>
       </c>
       <c r="G23" s="2">
         <f ca="1">F23+3</f>
-        <v>43641</v>
+        <v>43695</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>142</v>
@@ -8283,25 +8288,25 @@
       <c r="O23">
         <v>101</v>
       </c>
-      <c r="P23" t="str">
+      <c r="P23" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K23,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.009.QR_LIVE</v>
-      </c>
-      <c r="Q23" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q23" t="e">
         <f t="array" aca="1" ref="Q23:T24" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P23))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R23" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S23" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T23" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R23" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S23" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T23" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -8313,21 +8318,21 @@
       <c r="H24" s="2"/>
       <c r="I24" s="3"/>
       <c r="N24" s="7"/>
-      <c r="Q24" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R24" s="37">
-        <f ca="1"/>
-        <v>0.140197487625769</v>
-      </c>
-      <c r="S24" s="57">
-        <f ca="1"/>
-        <v>-949508.15758384624</v>
-      </c>
-      <c r="T24" s="57">
-        <f ca="1"/>
-        <v>-40768.314622856997</v>
+      <c r="Q24" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R24" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S24" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T24" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -8348,11 +8353,11 @@
       </c>
       <c r="F25" s="2">
         <f t="shared" ref="F25" ca="1" si="0">F23+2</f>
-        <v>43640</v>
+        <v>43694</v>
       </c>
       <c r="G25" s="2">
         <f ca="1">F25+3</f>
-        <v>43643</v>
+        <v>43697</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>142</v>
@@ -8379,43 +8384,43 @@
       <c r="O25">
         <v>101</v>
       </c>
-      <c r="P25" t="str">
+      <c r="P25" t="e">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K25,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.010.QR_LIVE</v>
-      </c>
-      <c r="Q25" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q25" t="e">
         <f t="array" aca="1" ref="Q25:T26" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P25))</f>
-        <v>YieldToMaturity</v>
-      </c>
-      <c r="R25" t="str">
-        <f ca="1"/>
-        <v>AssetSwapSpread</v>
-      </c>
-      <c r="S25" t="str">
-        <f ca="1"/>
-        <v>NPV</v>
-      </c>
-      <c r="T25" t="str">
-        <f ca="1"/>
-        <v>PandL</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R25" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S25" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T25" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="26" spans="1:20">
-      <c r="Q26" s="37">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="R26" s="37">
-        <f ca="1"/>
-        <v>0.140197487625769</v>
-      </c>
-      <c r="S26" s="57">
-        <f ca="1"/>
-        <v>-1055009.0639820513</v>
-      </c>
-      <c r="T26" s="57">
-        <f ca="1"/>
-        <v>-45298.127358729995</v>
+      <c r="Q26" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R26" s="37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S26" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T26" s="57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bond transactions now include coupon information.
</commit_message>
<xml_diff>
--- a/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/BondTransactionPricer.xlsx
+++ b/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/BondTransactionPricer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2019\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Product Pricers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0274AB-6446-40F1-BA6A-A2D3EF553DE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E518A6D-FF10-4AEE-9F84-0FD8D96AD2EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1410" yWindow="465" windowWidth="26370" windowHeight="14820" tabRatio="836" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1409,7 +1409,7 @@
     <xf numFmtId="38" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1661,6 +1661,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2180,20 +2181,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" thickBot="1">
-      <c r="A1" s="121" t="str">
+      <c r="A1" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( A2:B11, $C$18:$E$41)</f>
         <v>Market.QR_LIVE.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
-      <c r="B1" s="122"/>
+      <c r="B1" s="123"/>
       <c r="C1" s="80"/>
       <c r="D1" s="80"/>
       <c r="E1" s="80"/>
       <c r="F1" s="81"/>
-      <c r="G1" s="121" t="str">
+      <c r="G1" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G2:H12, $C$18:$E$41)</f>
-        <v>Market.QR_LIVE.2019-08-18.DiscountCurve.AUD-LIBOR-SENIOR</v>
-      </c>
-      <c r="H1" s="122"/>
+        <v>Market.QR_LIVE.2019-08-25.DiscountCurve.AUD-LIBOR-SENIOR</v>
+      </c>
+      <c r="H1" s="123"/>
       <c r="I1" s="81"/>
     </row>
     <row r="2" spans="1:9" ht="13.5" thickBot="1">
@@ -2221,7 +2222,7 @@
       </c>
       <c r="B3" s="85">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="C3" s="80"/>
       <c r="D3" s="80"/>
@@ -2232,7 +2233,7 @@
       </c>
       <c r="H3" s="85">
         <f ca="1">H6</f>
-        <v>43695</v>
+        <v>43702</v>
       </c>
       <c r="I3" s="84"/>
     </row>
@@ -2242,7 +2243,7 @@
       </c>
       <c r="B4" s="86">
         <f ca="1">B3</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="C4" s="80"/>
       <c r="D4" s="80"/>
@@ -2253,7 +2254,7 @@
       </c>
       <c r="H4" s="86">
         <f ca="1">H3</f>
-        <v>43695</v>
+        <v>43702</v>
       </c>
       <c r="I4" s="84"/>
     </row>
@@ -2292,7 +2293,7 @@
       </c>
       <c r="H6" s="88">
         <f ca="1">'BondCurve-BondForward'!G7</f>
-        <v>43695</v>
+        <v>43702</v>
       </c>
       <c r="I6" s="84"/>
     </row>
@@ -2435,11 +2436,11 @@
       <c r="D14" s="80"/>
       <c r="E14" s="80"/>
       <c r="F14" s="84"/>
-      <c r="G14" s="121" t="str">
+      <c r="G14" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G15:H25,HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-08-17.DiscountCurve.AUD-LIBOR-SENIOR</v>
-      </c>
-      <c r="H14" s="122"/>
+        <v>Market.QR_LIVE.2019-08-24.DiscountCurve.AUD-LIBOR-SENIOR</v>
+      </c>
+      <c r="H14" s="123"/>
       <c r="I14" s="84"/>
     </row>
     <row r="15" spans="1:9" ht="13.5" thickBot="1">
@@ -2471,7 +2472,7 @@
       </c>
       <c r="H16" s="85">
         <f ca="1">H19</f>
-        <v>43694</v>
+        <v>43701</v>
       </c>
       <c r="I16" s="84"/>
     </row>
@@ -2497,7 +2498,7 @@
       </c>
       <c r="H17" s="86">
         <f ca="1">H16</f>
-        <v>43694</v>
+        <v>43701</v>
       </c>
       <c r="I17" s="84"/>
     </row>
@@ -2550,7 +2551,7 @@
       </c>
       <c r="H19" s="88">
         <f ca="1">'BondCurve-BondForward'!G21</f>
-        <v>43694</v>
+        <v>43701</v>
       </c>
       <c r="I19" s="84"/>
     </row>
@@ -2750,11 +2751,11 @@
         <v>0</v>
       </c>
       <c r="F27" s="84"/>
-      <c r="G27" s="121" t="str">
+      <c r="G27" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G28:H38, HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-08-16.DiscountCurve.AUD-LIBOR-SENIOR</v>
-      </c>
-      <c r="H27" s="122"/>
+        <v>Market.QR_LIVE.2019-08-23.DiscountCurve.AUD-LIBOR-SENIOR</v>
+      </c>
+      <c r="H27" s="123"/>
       <c r="I27" s="84"/>
     </row>
     <row r="28" spans="1:9" ht="13.5" thickBot="1">
@@ -2806,7 +2807,7 @@
       </c>
       <c r="H29" s="85">
         <f ca="1">H32</f>
-        <v>43693</v>
+        <v>43700</v>
       </c>
       <c r="I29" s="84"/>
     </row>
@@ -2833,7 +2834,7 @@
       </c>
       <c r="H30" s="86">
         <f ca="1">H29</f>
-        <v>43693</v>
+        <v>43700</v>
       </c>
       <c r="I30" s="84"/>
     </row>
@@ -2886,7 +2887,7 @@
       </c>
       <c r="H32" s="88">
         <f ca="1">'BondCurve-BondForward'!G35</f>
-        <v>43693</v>
+        <v>43700</v>
       </c>
       <c r="I32" s="84"/>
     </row>
@@ -3086,11 +3087,11 @@
         <v>0</v>
       </c>
       <c r="F40" s="84"/>
-      <c r="G40" s="121" t="str">
+      <c r="G40" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G41:H51, HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-08-15.DiscountCurve.AUD-LIBOR-SENIOR</v>
-      </c>
-      <c r="H40" s="122"/>
+        <v>Market.QR_LIVE.2019-08-22.DiscountCurve.AUD-LIBOR-SENIOR</v>
+      </c>
+      <c r="H40" s="123"/>
       <c r="I40" s="84"/>
     </row>
     <row r="41" spans="1:9" ht="13.5" thickBot="1">
@@ -3131,7 +3132,7 @@
       </c>
       <c r="H42" s="85">
         <f ca="1">H45</f>
-        <v>43692</v>
+        <v>43699</v>
       </c>
       <c r="I42" s="84"/>
     </row>
@@ -3149,7 +3150,7 @@
       </c>
       <c r="H43" s="86">
         <f ca="1">H42</f>
-        <v>43692</v>
+        <v>43699</v>
       </c>
       <c r="I43" s="84"/>
     </row>
@@ -3180,7 +3181,7 @@
       </c>
       <c r="H45" s="88">
         <f ca="1">'BondCurve-BondForward'!G49</f>
-        <v>43692</v>
+        <v>43699</v>
       </c>
       <c r="I45" s="82"/>
     </row>
@@ -3235,11 +3236,11 @@
       </c>
     </row>
     <row r="53" spans="7:8" ht="13.5" thickBot="1">
-      <c r="G53" s="121" t="str">
+      <c r="G53" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G54:H64, HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-08-14.DiscountCurve.AUD-LIBOR-SENIOR</v>
-      </c>
-      <c r="H53" s="122"/>
+        <v>Market.QR_LIVE.2019-08-21.DiscountCurve.AUD-LIBOR-SENIOR</v>
+      </c>
+      <c r="H53" s="123"/>
     </row>
     <row r="54" spans="7:8" ht="13.5" thickBot="1">
       <c r="G54" s="19" t="s">
@@ -3255,7 +3256,7 @@
       </c>
       <c r="H55" s="85">
         <f ca="1">H58</f>
-        <v>43691</v>
+        <v>43698</v>
       </c>
     </row>
     <row r="56" spans="7:8">
@@ -3264,7 +3265,7 @@
       </c>
       <c r="H56" s="86">
         <f ca="1">H55</f>
-        <v>43691</v>
+        <v>43698</v>
       </c>
     </row>
     <row r="57" spans="7:8">
@@ -3281,7 +3282,7 @@
       </c>
       <c r="H58" s="88">
         <f ca="1">'BondCurve-BondForward'!G63</f>
-        <v>43691</v>
+        <v>43698</v>
       </c>
     </row>
     <row r="59" spans="7:8">
@@ -3386,11 +3387,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="13.5" thickBot="1">
-      <c r="B2" s="123" t="str">
+      <c r="B2" s="124" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(B3:C13, B17:D21)</f>
         <v>Market.QR_LIVE.DiscountCurve.AUD-WATC-SENIOR</v>
       </c>
-      <c r="C2" s="124"/>
+      <c r="C2" s="125"/>
     </row>
     <row r="3" spans="2:4" ht="13.5" thickBot="1">
       <c r="B3" s="19" t="s">
@@ -3406,7 +3407,7 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -3415,7 +3416,7 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -3771,16 +3772,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="13.5" thickBot="1">
-      <c r="B2" s="123" t="str">
+      <c r="B2" s="124" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(B3:C14, B18:D21)</f>
         <v>Market.QR_LIVE.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="F2" s="123" t="str">
+      <c r="C2" s="125"/>
+      <c r="F2" s="124" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F3:G15, $B$18:$D$21)</f>
-        <v>Market.QR_LIVE.2019-08-18.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
-      </c>
-      <c r="G2" s="124"/>
+        <v>Market.QR_LIVE.2019-08-25.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+      </c>
+      <c r="G2" s="125"/>
     </row>
     <row r="3" spans="2:9" ht="13.5" thickBot="1">
       <c r="B3" s="19" t="s">
@@ -3802,14 +3803,14 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="25">
         <f ca="1">G7</f>
-        <v>43695</v>
+        <v>43702</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -3818,14 +3819,14 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="26">
         <f ca="1">G4</f>
-        <v>43695</v>
+        <v>43702</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -3843,7 +3844,7 @@
       </c>
       <c r="I6" t="str">
         <f ca="1">G6&amp;"."&amp;TEXT(G7,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-18</v>
+        <v>QR_LIVE.2019-08-25</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -3858,11 +3859,11 @@
       </c>
       <c r="G7" s="77">
         <f ca="1">$C$5-1</f>
-        <v>43695</v>
+        <v>43702</v>
       </c>
       <c r="I7" t="str">
         <f ca="1">G20&amp;"."&amp;TEXT(G21,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-17</v>
+        <v>QR_LIVE.2019-08-24</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -3880,7 +3881,7 @@
       </c>
       <c r="I8" t="str">
         <f ca="1">G34&amp;"."&amp;TEXT(G35,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-16</v>
+        <v>QR_LIVE.2019-08-23</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -3898,7 +3899,7 @@
       </c>
       <c r="I9" t="str">
         <f ca="1">G48&amp;"."&amp;TEXT(G49,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-15</v>
+        <v>QR_LIVE.2019-08-22</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -3916,7 +3917,7 @@
       </c>
       <c r="I10" t="str">
         <f ca="1">G62&amp;"."&amp;TEXT(G63,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-14</v>
+        <v>QR_LIVE.2019-08-21</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -3987,11 +3988,11 @@
       <c r="B16" s="33"/>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
-      <c r="F16" s="125" t="str">
+      <c r="F16" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F17:G29, $B$23:$D$26)</f>
-        <v>Market.QR_LIVE.2019-08-17.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
-      </c>
-      <c r="G16" s="126"/>
+        <v>Market.QR_LIVE.2019-08-24.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+      </c>
+      <c r="G16" s="127"/>
     </row>
     <row r="17" spans="2:7" ht="13.5" thickBot="1">
       <c r="B17" s="33" t="s">
@@ -4025,7 +4026,7 @@
       </c>
       <c r="G18" s="25">
         <f ca="1">G21</f>
-        <v>43694</v>
+        <v>43701</v>
       </c>
     </row>
     <row r="19" spans="2:7">
@@ -4043,7 +4044,7 @@
       </c>
       <c r="G19" s="26">
         <f ca="1">G18</f>
-        <v>43694</v>
+        <v>43701</v>
       </c>
     </row>
     <row r="20" spans="2:7">
@@ -4079,7 +4080,7 @@
       </c>
       <c r="G21" s="77">
         <f ca="1">$G$7-1</f>
-        <v>43694</v>
+        <v>43701</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="13.5" thickBot="1">
@@ -4210,11 +4211,11 @@
       <c r="D30" s="17">
         <v>0</v>
       </c>
-      <c r="F30" s="125" t="str">
+      <c r="F30" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F31:G43, $B$28:$D$31)</f>
-        <v>Market.QR_LIVE.2019-08-16.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
-      </c>
-      <c r="G30" s="126"/>
+        <v>Market.QR_LIVE.2019-08-23.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+      </c>
+      <c r="G30" s="127"/>
     </row>
     <row r="31" spans="2:7" ht="13.5" thickBot="1">
       <c r="B31" s="70" t="s">
@@ -4239,7 +4240,7 @@
       </c>
       <c r="G32" s="25">
         <f ca="1">G35</f>
-        <v>43693</v>
+        <v>43700</v>
       </c>
     </row>
     <row r="33" spans="2:7">
@@ -4257,7 +4258,7 @@
       </c>
       <c r="G33" s="26">
         <f ca="1">G32</f>
-        <v>43693</v>
+        <v>43700</v>
       </c>
     </row>
     <row r="34" spans="2:7">
@@ -4293,7 +4294,7 @@
       </c>
       <c r="G35" s="77">
         <f ca="1">$G$7-2</f>
-        <v>43693</v>
+        <v>43700</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="13.5" thickBot="1">
@@ -4409,11 +4410,11 @@
       <c r="B44" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="F44" s="125" t="str">
+      <c r="F44" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F45:G57, $B$33:$D$36)</f>
-        <v>Market.QR_LIVE.2019-08-15.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
-      </c>
-      <c r="G44" s="126"/>
+        <v>Market.QR_LIVE.2019-08-22.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+      </c>
+      <c r="G44" s="127"/>
     </row>
     <row r="45" spans="2:7" ht="13.5" thickBot="1">
       <c r="B45" s="68" t="str">
@@ -4445,7 +4446,7 @@
       </c>
       <c r="G46" s="25">
         <f ca="1">G49</f>
-        <v>43692</v>
+        <v>43699</v>
       </c>
     </row>
     <row r="47" spans="2:7">
@@ -4462,7 +4463,7 @@
       </c>
       <c r="G47" s="26">
         <f ca="1">G46</f>
-        <v>43692</v>
+        <v>43699</v>
       </c>
     </row>
     <row r="48" spans="2:7">
@@ -4496,7 +4497,7 @@
       </c>
       <c r="G49" s="77">
         <f ca="1">$G$7-3</f>
-        <v>43692</v>
+        <v>43699</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="13.5" thickBot="1">
@@ -4521,7 +4522,7 @@
     <row r="52" spans="2:7">
       <c r="B52" s="73">
         <f t="array" aca="1" ref="B52:C56" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="C52" s="30">
         <f ca="1"/>
@@ -4537,7 +4538,7 @@
     <row r="53" spans="2:7">
       <c r="B53" s="74">
         <f ca="1"/>
-        <v>43698</v>
+        <v>43705</v>
       </c>
       <c r="C53" s="31">
         <f ca="1"/>
@@ -4553,7 +4554,7 @@
     <row r="54" spans="2:7">
       <c r="B54" s="74">
         <f ca="1"/>
-        <v>43731</v>
+        <v>43738</v>
       </c>
       <c r="C54" s="31">
         <f ca="1"/>
@@ -4569,7 +4570,7 @@
     <row r="55" spans="2:7">
       <c r="B55" s="74">
         <f ca="1"/>
-        <v>43759</v>
+        <v>43766</v>
       </c>
       <c r="C55" s="31">
         <f ca="1"/>
@@ -4610,16 +4611,16 @@
       <c r="B58" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="F58" s="125" t="str">
+      <c r="F58" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F59:G71, $B$38:$D$41)</f>
-        <v>Market.QR_LIVE.2019-08-14.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
-      </c>
-      <c r="G58" s="126"/>
+        <v>Market.QR_LIVE.2019-08-21.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+      </c>
+      <c r="G58" s="127"/>
     </row>
     <row r="59" spans="2:7" ht="13.5" thickBot="1">
       <c r="B59" s="73">
         <f ca="1">B52</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="C59" s="30">
         <f t="array" aca="1" ref="C59:C63" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B52:B56)</f>
@@ -4635,7 +4636,7 @@
     <row r="60" spans="2:7">
       <c r="B60" s="74">
         <f t="shared" ref="B60:B63" ca="1" si="0">B53</f>
-        <v>43698</v>
+        <v>43705</v>
       </c>
       <c r="C60" s="31">
         <f ca="1"/>
@@ -4646,13 +4647,13 @@
       </c>
       <c r="G60" s="25">
         <f ca="1">G63</f>
-        <v>43691</v>
+        <v>43698</v>
       </c>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43731</v>
+        <v>43738</v>
       </c>
       <c r="C61" s="31">
         <f ca="1"/>
@@ -4663,13 +4664,13 @@
       </c>
       <c r="G61" s="26">
         <f ca="1">G60</f>
-        <v>43691</v>
+        <v>43698</v>
       </c>
     </row>
     <row r="62" spans="2:7">
       <c r="B62" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43759</v>
+        <v>43766</v>
       </c>
       <c r="C62" s="31">
         <f ca="1"/>
@@ -4697,7 +4698,7 @@
       </c>
       <c r="G63" s="77">
         <f ca="1">$G$7-4</f>
-        <v>43691</v>
+        <v>43698</v>
       </c>
     </row>
     <row r="64" spans="2:7">
@@ -4795,11 +4796,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="13.5" thickBot="1">
-      <c r="B2" s="123" t="str">
+      <c r="B2" s="124" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(B3:C15, B19:D22)</f>
         <v>Market.QR_LIVE.RateCurve.AUD-WATC-SECURED</v>
       </c>
-      <c r="C2" s="124"/>
+      <c r="C2" s="125"/>
     </row>
     <row r="3" spans="2:3" ht="13.5" thickBot="1">
       <c r="B3" s="19" t="s">
@@ -4815,7 +4816,7 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -4824,7 +4825,7 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -5032,7 +5033,7 @@
     <row r="32" spans="2:4">
       <c r="B32" s="73">
         <f t="array" aca="1" ref="B32:C36" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="C32" s="30">
         <f ca="1"/>
@@ -5042,7 +5043,7 @@
     <row r="33" spans="2:3">
       <c r="B33" s="74">
         <f ca="1"/>
-        <v>43697</v>
+        <v>43704</v>
       </c>
       <c r="C33" s="31">
         <f ca="1"/>
@@ -5052,7 +5053,7 @@
     <row r="34" spans="2:3">
       <c r="B34" s="74">
         <f ca="1"/>
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="C34" s="31">
         <f ca="1"/>
@@ -5062,7 +5063,7 @@
     <row r="35" spans="2:3">
       <c r="B35" s="74">
         <f ca="1"/>
-        <v>43759</v>
+        <v>43766</v>
       </c>
       <c r="C35" s="31">
         <f ca="1"/>
@@ -5072,7 +5073,7 @@
     <row r="36" spans="2:3" ht="13.5" thickBot="1">
       <c r="B36" s="75">
         <f ca="1"/>
-        <v>43789</v>
+        <v>43796</v>
       </c>
       <c r="C36" s="32">
         <f ca="1"/>
@@ -5088,7 +5089,7 @@
     <row r="39" spans="2:3">
       <c r="B39" s="73">
         <f ca="1">B32</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="C39" s="30">
         <f t="array" aca="1" ref="C39:C43" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B32:B36)</f>
@@ -5098,7 +5099,7 @@
     <row r="40" spans="2:3">
       <c r="B40" s="74">
         <f t="shared" ref="B40:B43" ca="1" si="0">B33</f>
-        <v>43697</v>
+        <v>43704</v>
       </c>
       <c r="C40" s="31">
         <f ca="1"/>
@@ -5108,7 +5109,7 @@
     <row r="41" spans="2:3">
       <c r="B41" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="C41" s="31">
         <f ca="1"/>
@@ -5118,7 +5119,7 @@
     <row r="42" spans="2:3">
       <c r="B42" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43759</v>
+        <v>43766</v>
       </c>
       <c r="C42" s="31">
         <f ca="1"/>
@@ -5128,7 +5129,7 @@
     <row r="43" spans="2:3" ht="13.5" thickBot="1">
       <c r="B43" s="75">
         <f t="shared" ca="1" si="0"/>
-        <v>43789</v>
+        <v>43796</v>
       </c>
       <c r="C43" s="32">
         <f ca="1"/>
@@ -5189,16 +5190,16 @@
       </c>
     </row>
     <row r="2" spans="2:7" ht="13.5" thickBot="1">
-      <c r="B2" s="123" t="str">
+      <c r="B2" s="124" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(B3:C17, $B$21:$D$24)</f>
         <v>Market.QR_LIVE.2014-03-21.RateCurve.AUD-GC-SECURED</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="F2" s="123" t="str">
+      <c r="C2" s="125"/>
+      <c r="F2" s="124" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F3:G17, $B$21:$D$24)</f>
         <v>Market.QR_LIVE.2014-03-20.RateCurve.AUD-GC-SECURED</v>
       </c>
-      <c r="G2" s="124"/>
+      <c r="G2" s="125"/>
     </row>
     <row r="3" spans="2:7" ht="13.5" thickBot="1">
       <c r="B3" s="19" t="s">
@@ -5220,14 +5221,14 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="25">
         <f ca="1">G5</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -5236,14 +5237,14 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -5417,11 +5418,11 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="13.5" thickBot="1">
-      <c r="F18" s="125" t="str">
+      <c r="F18" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F19:G33, $B$21:$D$24)</f>
         <v>Market.QR_LIVE.2014-03-19.RateCurve.AUD-GC-SECURED</v>
       </c>
-      <c r="G18" s="126"/>
+      <c r="G18" s="127"/>
     </row>
     <row r="19" spans="2:7" ht="13.5" thickBot="1">
       <c r="B19" s="33"/>
@@ -5451,7 +5452,7 @@
       </c>
       <c r="G20" s="25">
         <f ca="1">G21</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -5470,7 +5471,7 @@
       </c>
       <c r="G21" s="26">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="22" spans="2:7">
@@ -5603,7 +5604,7 @@
       </c>
       <c r="C30" s="65">
         <f ca="1"/>
-        <v>5.0006783133467556E-2</v>
+        <v>5.0006791423151439E-2</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>38</v>
@@ -5650,22 +5651,22 @@
     <row r="34" spans="2:7" ht="13.5" thickBot="1">
       <c r="B34" s="73">
         <f t="array" aca="1" ref="B34:C38" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="C34" s="64">
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="F34" s="125" t="str">
+      <c r="F34" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F35:G49, $B$21:$D$24)</f>
         <v>Market.QR_LIVE.2014-03-18.RateCurve.AUD-GC-SECURED</v>
       </c>
-      <c r="G34" s="126"/>
+      <c r="G34" s="127"/>
     </row>
     <row r="35" spans="2:7" ht="13.5" thickBot="1">
       <c r="B35" s="74">
         <f ca="1"/>
-        <v>43697</v>
+        <v>43704</v>
       </c>
       <c r="C35" s="65">
         <f ca="1"/>
@@ -5681,7 +5682,7 @@
     <row r="36" spans="2:7">
       <c r="B36" s="74">
         <f ca="1"/>
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="C36" s="65">
         <f ca="1"/>
@@ -5692,13 +5693,13 @@
       </c>
       <c r="G36" s="25">
         <f ca="1">G37</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="74">
         <f ca="1"/>
-        <v>43759</v>
+        <v>43766</v>
       </c>
       <c r="C37" s="65">
         <f ca="1"/>
@@ -5709,17 +5710,17 @@
       </c>
       <c r="G37" s="26">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="13.5" thickBot="1">
       <c r="B38" s="75">
         <f ca="1"/>
-        <v>43789</v>
+        <v>43796</v>
       </c>
       <c r="C38" s="66">
         <f ca="1"/>
-        <v>0.98741718250559696</v>
+        <v>0.987417180468115</v>
       </c>
       <c r="F38" s="22" t="s">
         <v>26</v>
@@ -5752,7 +5753,7 @@
     <row r="41" spans="2:7">
       <c r="B41" s="73">
         <f ca="1">B34</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="C41" s="64">
         <f t="array" aca="1" ref="C41:C45" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B34:B38)</f>
@@ -5768,7 +5769,7 @@
     <row r="42" spans="2:7">
       <c r="B42" s="74">
         <f t="shared" ref="B42:B45" ca="1" si="0">B35</f>
-        <v>43697</v>
+        <v>43704</v>
       </c>
       <c r="C42" s="65">
         <f ca="1"/>
@@ -5784,7 +5785,7 @@
     <row r="43" spans="2:7">
       <c r="B43" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="C43" s="65">
         <f ca="1"/>
@@ -5800,7 +5801,7 @@
     <row r="44" spans="2:7">
       <c r="B44" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43759</v>
+        <v>43766</v>
       </c>
       <c r="C44" s="65">
         <f ca="1"/>
@@ -5816,11 +5817,11 @@
     <row r="45" spans="2:7" ht="13.5" thickBot="1">
       <c r="B45" s="75">
         <f t="shared" ca="1" si="0"/>
-        <v>43789</v>
+        <v>43796</v>
       </c>
       <c r="C45" s="66">
         <f ca="1"/>
-        <v>5.0007516164302303E-2</v>
+        <v>5.0007524364018799E-2</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>37</v>
@@ -5870,11 +5871,11 @@
     <row r="50" spans="2:7" ht="13.5" thickBot="1">
       <c r="B50" s="76"/>
       <c r="C50" s="67"/>
-      <c r="F50" s="125" t="str">
+      <c r="F50" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F51:G65, $B$21:$D$24)</f>
         <v>Market.QR_LIVE.2014-03-17.RateCurve.AUD-GC-SECURED</v>
       </c>
-      <c r="G50" s="126"/>
+      <c r="G50" s="127"/>
     </row>
     <row r="51" spans="2:7" ht="13.5" thickBot="1">
       <c r="B51" s="76"/>
@@ -5892,7 +5893,7 @@
       </c>
       <c r="G52" s="25">
         <f ca="1">G53</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="53" spans="2:7">
@@ -5901,7 +5902,7 @@
       </c>
       <c r="G53" s="26">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
     </row>
     <row r="54" spans="2:7">
@@ -6017,10 +6018,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:I45"/>
+  <dimension ref="B1:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6031,38 +6032,143 @@
     <col min="4" max="4" width="4.28515625" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
     <col min="8" max="8" width="84.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9">
+    <row r="1" spans="2:22">
       <c r="F1" t="str">
         <f t="array" ref="F1:F13">_xll.HLV5r3.Financial.Cache.SupportedBondMetrics()</f>
         <v>DirtyPrice</v>
       </c>
-      <c r="H1" s="1" t="e">
+      <c r="H1" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I1,$C$10)</f>
-        <v>#VALUE!</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE</v>
       </c>
       <c r="I1" t="str">
         <f>'BondCurve-BondForward'!C6</f>
         <v>QR_LIVE</v>
       </c>
-    </row>
-    <row r="2" spans="2:9">
+      <c r="K1" t="str">
+        <f t="array" aca="1" ref="K1:V11" ca="1">_xll.HLV5r3.Financial.Cache.ViewExpectedCashFlows(B22,C18,E3:E7,C27,$I$1,C16)</f>
+        <v>Trade.SpreadSheet.bondTransaction.testtrade_001</v>
+      </c>
+      <c r="L1" t="str">
+        <f ca="1"/>
+        <v>PrincipalExchange</v>
+      </c>
+      <c r="M1">
+        <f ca="1"/>
+        <v>43708</v>
+      </c>
+      <c r="N1" t="str">
+        <f ca="1"/>
+        <v>AUD</v>
+      </c>
+      <c r="O1">
+        <f ca="1"/>
+        <v>-101000000</v>
+      </c>
+      <c r="P1" t="str">
+        <f ca="1"/>
+        <v>DiscountedCashflow</v>
+      </c>
+      <c r="Q1">
+        <f ca="1"/>
+        <v>0.99931544357534796</v>
+      </c>
+      <c r="R1">
+        <f ca="1"/>
+        <v>-100930859.80111015</v>
+      </c>
+      <c r="S1">
+        <f ca="1"/>
+        <v>1.3698630136986301E-2</v>
+      </c>
+      <c r="T1" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="U1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="V1" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22">
       <c r="F2" t="str">
         <v>CleanPrice</v>
       </c>
-      <c r="H2" s="1" t="e">
+      <c r="H2" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I2,$C$10)</f>
-        <v>#VALUE!</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-25</v>
       </c>
       <c r="I2" t="str">
         <f ca="1">'BondCurve-BondForward'!I6</f>
-        <v>QR_LIVE.2019-08-18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9">
+        <v>QR_LIVE.2019-08-25</v>
+      </c>
+      <c r="K2" t="str">
+        <f ca="1"/>
+        <v>Trade.SpreadSheet.bondTransaction.testtrade_001</v>
+      </c>
+      <c r="L2" t="str">
+        <f ca="1"/>
+        <v>PrincipalExchange</v>
+      </c>
+      <c r="M2">
+        <f ca="1"/>
+        <v>43753</v>
+      </c>
+      <c r="N2" t="str">
+        <f ca="1"/>
+        <v>AUD</v>
+      </c>
+      <c r="O2">
+        <f ca="1"/>
+        <v>100000000</v>
+      </c>
+      <c r="P2" t="str">
+        <f ca="1"/>
+        <v>DiscountedCashflow</v>
+      </c>
+      <c r="Q2">
+        <f ca="1"/>
+        <v>0.99319547997258495</v>
+      </c>
+      <c r="R2">
+        <f ca="1"/>
+        <v>99319547.997258514</v>
+      </c>
+      <c r="S2">
+        <f ca="1"/>
+        <v>0.13698630136986301</v>
+      </c>
+      <c r="T2" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="U2" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="V2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -6075,16 +6181,64 @@
       <c r="F3" t="str">
         <v>NPV</v>
       </c>
-      <c r="H3" s="1" t="e">
+      <c r="H3" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I3,$C$10)</f>
-        <v>#VALUE!</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-24</v>
       </c>
       <c r="I3" t="str">
         <f ca="1">'BondCurve-BondForward'!I7</f>
-        <v>QR_LIVE.2019-08-17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
+        <v>QR_LIVE.2019-08-24</v>
+      </c>
+      <c r="K3" t="str">
+        <f ca="1"/>
+        <v>Trade.SpreadSheet.bondTransaction.testtrade_001</v>
+      </c>
+      <c r="L3" t="str">
+        <f ca="1"/>
+        <v>Coupon</v>
+      </c>
+      <c r="M3">
+        <f ca="1"/>
+        <v>43570</v>
+      </c>
+      <c r="N3" t="str">
+        <f ca="1"/>
+        <v>AUD</v>
+      </c>
+      <c r="O3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="P3" t="str">
+        <f ca="1"/>
+        <v>FixedRateRateCoupon</v>
+      </c>
+      <c r="Q3">
+        <f ca="1"/>
+        <v>1.0183848891398799</v>
+      </c>
+      <c r="R3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f ca="1"/>
+        <v>-0.36438356164383601</v>
+      </c>
+      <c r="T3" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="V3" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -6097,16 +6251,64 @@
       <c r="F4" t="str">
         <v>AccruedInterest</v>
       </c>
-      <c r="H4" s="1" t="e">
+      <c r="H4" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I4,$C$10)</f>
-        <v>#VALUE!</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-23</v>
       </c>
       <c r="I4" t="str">
         <f ca="1">'BondCurve-BondForward'!I8</f>
-        <v>QR_LIVE.2019-08-16</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
+        <v>QR_LIVE.2019-08-23</v>
+      </c>
+      <c r="K4" t="str">
+        <f ca="1"/>
+        <v>Trade.SpreadSheet.bondTransaction.testtrade_001</v>
+      </c>
+      <c r="L4" t="str">
+        <f ca="1"/>
+        <v>Coupon</v>
+      </c>
+      <c r="M4">
+        <f ca="1"/>
+        <v>43753</v>
+      </c>
+      <c r="N4" t="str">
+        <f ca="1"/>
+        <v>AUD</v>
+      </c>
+      <c r="O4">
+        <f ca="1"/>
+        <v>3509589.0410958929</v>
+      </c>
+      <c r="P4" t="str">
+        <f ca="1"/>
+        <v>FixedRateRateCoupon</v>
+      </c>
+      <c r="Q4">
+        <f ca="1"/>
+        <v>0.99319547997258495</v>
+      </c>
+      <c r="R4">
+        <f ca="1"/>
+        <v>3485707.9721777597</v>
+      </c>
+      <c r="S4">
+        <f ca="1"/>
+        <v>0.13698630136986301</v>
+      </c>
+      <c r="T4" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="U4" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="V4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -6119,16 +6321,64 @@
       <c r="F5" t="str">
         <v>ImpliedQuote</v>
       </c>
-      <c r="H5" s="1" t="e">
+      <c r="H5" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I5,$C$10)</f>
-        <v>#VALUE!</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-22</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">'BondCurve-BondForward'!I9</f>
-        <v>QR_LIVE.2019-08-15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
+        <v>QR_LIVE.2019-08-22</v>
+      </c>
+      <c r="K5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -6141,24 +6391,122 @@
       <c r="F6" t="str">
         <v>Convexity</v>
       </c>
-      <c r="H6" s="1" t="e">
+      <c r="H6" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I6,$C$10)</f>
-        <v>#VALUE!</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-21</v>
       </c>
       <c r="I6" t="str">
         <f ca="1">'BondCurve-BondForward'!I10</f>
-        <v>QR_LIVE.2019-08-14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9">
+        <v>QR_LIVE.2019-08-21</v>
+      </c>
+      <c r="K6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22">
       <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F7" t="str">
         <v>DeltaR</v>
       </c>
-    </row>
-    <row r="8" spans="2:9">
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="K7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22">
       <c r="B8" t="s">
         <v>141</v>
       </c>
@@ -6168,8 +6516,58 @@
       <c r="F8" t="str">
         <v>DV01</v>
       </c>
-    </row>
-    <row r="9" spans="2:9">
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="K8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -6179,32 +6577,176 @@
       <c r="F9" t="str">
         <v>MarketQuote</v>
       </c>
-    </row>
-    <row r="10" spans="2:9">
+      <c r="K9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="F10" t="str">
         <v>AssetSwapSpread</v>
       </c>
-    </row>
-    <row r="11" spans="2:9">
+      <c r="K10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22">
       <c r="B11" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="2">
         <f ca="1">C10+5</f>
-        <v>43701</v>
+        <v>43708</v>
       </c>
       <c r="F11" t="str">
         <v>ZSpread</v>
       </c>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="K11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -6215,7 +6757,7 @@
         <v>YieldToMaturity</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:22">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -6229,7 +6771,7 @@
         <v>PandL</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:22">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -6240,7 +6782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:22">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -6248,21 +6790,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:22">
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="2">
         <f ca="1">C10</f>
-        <v>43696</v>
-      </c>
-      <c r="E16" t="e">
+        <v>43703</v>
+      </c>
+      <c r="E16" t="str">
         <f t="array" aca="1" ref="E16:F22" ca="1">_xll.HLV5r3.Financial.Cache.ViewValuationReport(H1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F16" s="60" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="F16" s="60">
+        <f ca="1"/>
+        <v>1.0622265512299201E-3</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -6272,13 +6814,13 @@
       <c r="C17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E17" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F17" s="60" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E17" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="F17" s="60">
+        <f ca="1"/>
+        <v>-0.12454490731241699</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -6288,13 +6830,13 @@
       <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="115" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E18" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="F18" s="115">
+        <f ca="1"/>
+        <v>108954135.48004666</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -6304,13 +6846,13 @@
       <c r="C19" t="s">
         <v>1</v>
       </c>
-      <c r="E19" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F19" s="115" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E19" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
+      </c>
+      <c r="F19" s="115">
+        <f ca="1"/>
+        <v>106987187.891278</v>
       </c>
     </row>
     <row r="20" spans="2:6">
@@ -6320,13 +6862,13 @@
       <c r="C20" t="s">
         <v>49</v>
       </c>
-      <c r="E20" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F20" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E20" t="str">
+        <f ca="1"/>
+        <v>DirtyPrice</v>
+      </c>
+      <c r="F20">
+        <f ca="1"/>
+        <v>1.0698718789127799</v>
       </c>
     </row>
     <row r="21" spans="2:6">
@@ -6336,28 +6878,28 @@
       <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="E21" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F21" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E21" t="str">
+        <f ca="1"/>
+        <v>AccrualFactor</v>
+      </c>
+      <c r="F21">
+        <f ca="1"/>
+        <v>10057.556785162775</v>
       </c>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="127" t="str">
+      <c r="B22" s="128" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateBondTrade(C13,C12,C18,C19,C17,C10,C11,C9,B3:B6,C3:C6,C20,C8)</f>
         <v>Trade.SpreadSheet.bondTransaction.testtrade_001</v>
       </c>
-      <c r="C22" s="127"/>
-      <c r="E22" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F22" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="C22" s="128"/>
+      <c r="E22" t="str">
+        <f ca="1"/>
+        <v>FloatingNPV</v>
+      </c>
+      <c r="F22">
+        <f ca="1"/>
+        <v>5089664.6875904994</v>
       </c>
     </row>
     <row r="24" spans="2:6">
@@ -6368,10 +6910,6 @@
       <c r="C24" t="str">
         <f ca="1"/>
         <v>Party1</v>
-      </c>
-      <c r="E24" t="e">
-        <f t="array" aca="1" ref="E24" ca="1">_xll.HLV5r3.Financial.Cache.ViewExpectedCashFlows(B22,C18,E3:E7,C27,$I$1,C16)</f>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="2:6">
@@ -6598,7 +7136,7 @@
   <dimension ref="B1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6722,7 +7260,7 @@
       </c>
       <c r="C10" s="2">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="E10" s="114" t="s">
         <v>140</v>
@@ -6740,7 +7278,7 @@
       </c>
       <c r="C11" s="2">
         <f ca="1">C10+5</f>
-        <v>43701</v>
+        <v>43708</v>
       </c>
       <c r="H11" t="str">
         <v>ZSpread</v>
@@ -6796,7 +7334,7 @@
       </c>
       <c r="C16" s="2">
         <f ca="1">C10</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="E16" s="61" t="str">
         <f t="array" ref="E16:F22">_xll.HLV5r3.Financial.Cache.ViewValuationReport(E27)</f>
@@ -6964,13 +7502,13 @@
         <f ca="1"/>
         <v>Fixed</v>
       </c>
-      <c r="E29" s="1" t="e">
+      <c r="E29" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarkets($C$22,$E$24,$C$18,$E$3:$E$7,"AUD",$H$29:$H$33,$C$10)</f>
-        <v>#VALUE!</v>
+        <v>Var_Run_20170531</v>
       </c>
       <c r="H29" s="1" t="str">
         <f t="array" aca="1" ref="H29:H33" ca="1">Markets</f>
-        <v>QR_LIVE.2019-08-18</v>
+        <v>QR_LIVE.2019-08-25</v>
       </c>
     </row>
     <row r="30" spans="2:8">
@@ -6984,7 +7522,7 @@
       </c>
       <c r="H30" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-08-17</v>
+        <v>QR_LIVE.2019-08-24</v>
       </c>
     </row>
     <row r="31" spans="2:8">
@@ -6998,7 +7536,7 @@
       </c>
       <c r="H31" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-08-16</v>
+        <v>QR_LIVE.2019-08-23</v>
       </c>
     </row>
     <row r="32" spans="2:8">
@@ -7019,7 +7557,7 @@
       </c>
       <c r="H32" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-08-15</v>
+        <v>QR_LIVE.2019-08-22</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -7039,7 +7577,7 @@
       </c>
       <c r="H33" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-08-14</v>
+        <v>QR_LIVE.2019-08-21</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -7330,7 +7868,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7356,23 +7894,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="39" customHeight="1">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="129" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
       <c r="P1" s="116"/>
     </row>
     <row r="2" spans="1:20">
@@ -7393,7 +7931,7 @@
       </c>
       <c r="K3" s="50">
         <f ca="1">TODAY()</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>21</v>
@@ -7502,11 +8040,11 @@
       </c>
       <c r="F7" s="2">
         <f ca="1">TODAY()-20</f>
-        <v>43676</v>
+        <v>43683</v>
       </c>
       <c r="G7" s="2">
         <f ca="1">F7+3</f>
-        <v>43679</v>
+        <v>43686</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>142</v>
@@ -7533,43 +8071,43 @@
       <c r="O7">
         <v>101</v>
       </c>
-      <c r="P7" t="e">
+      <c r="P7" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K7,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q7" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.001.QR_LIVE</v>
+      </c>
+      <c r="Q7" t="str">
         <f t="array" aca="1" ref="Q7:T8" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P7))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R7" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S7" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T7" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R7" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S7" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T7" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="Q8" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R8" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S8" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T8" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q8" s="37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R8" s="37">
+        <f ca="1"/>
+        <v>0.14928664798605062</v>
+      </c>
+      <c r="S8" s="57">
+        <f ca="1"/>
+        <v>95392.978256669478</v>
+      </c>
+      <c r="T8" s="57">
+        <f ca="1"/>
+        <v>93670.850062629703</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -7590,11 +8128,11 @@
       </c>
       <c r="F9" s="2">
         <f ca="1">F7+2</f>
-        <v>43678</v>
+        <v>43685</v>
       </c>
       <c r="G9" s="2">
         <f ca="1">F9+3</f>
-        <v>43681</v>
+        <v>43688</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>142</v>
@@ -7621,25 +8159,25 @@
       <c r="O9">
         <v>101</v>
       </c>
-      <c r="P9" t="e">
+      <c r="P9" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K9,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q9" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.002.QR_LIVE</v>
+      </c>
+      <c r="Q9" t="str">
         <f t="array" aca="1" ref="Q9:T10" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P9))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R9" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S9" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T9" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -7651,21 +8189,21 @@
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
       <c r="N10" s="7"/>
-      <c r="Q10" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R10" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S10" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T10" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q10" s="37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R10" s="37">
+        <f ca="1"/>
+        <v>0.13204488198804987</v>
+      </c>
+      <c r="S10" s="57">
+        <f ca="1"/>
+        <v>192493.7092904264</v>
+      </c>
+      <c r="T10" s="57">
+        <f ca="1"/>
+        <v>189018.6228637044</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -7686,11 +8224,11 @@
       </c>
       <c r="F11" s="2">
         <f ca="1">F9+2</f>
-        <v>43680</v>
+        <v>43687</v>
       </c>
       <c r="G11" s="2">
         <f ca="1">F11+3</f>
-        <v>43683</v>
+        <v>43690</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>142</v>
@@ -7717,25 +8255,25 @@
       <c r="O11">
         <v>101</v>
       </c>
-      <c r="P11" t="e">
+      <c r="P11" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K11,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q11" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.003.QR_LIVE</v>
+      </c>
+      <c r="Q11" t="str">
         <f t="array" aca="1" ref="Q11:T12" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P11))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R11" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S11" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T11" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R11" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S11" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T11" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -7747,21 +8285,21 @@
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
       <c r="N12" s="7"/>
-      <c r="Q12" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R12" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S12" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T12" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q12" s="37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R12" s="37">
+        <f ca="1"/>
+        <v>0.12771037962458848</v>
+      </c>
+      <c r="S12" s="57">
+        <f ca="1"/>
+        <v>289384.54597750399</v>
+      </c>
+      <c r="T12" s="57">
+        <f ca="1"/>
+        <v>284160.29053800664</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -7782,11 +8320,11 @@
       </c>
       <c r="F13" s="2">
         <f ca="1">F11+2</f>
-        <v>43682</v>
+        <v>43689</v>
       </c>
       <c r="G13" s="2">
         <f ca="1">F13+3</f>
-        <v>43685</v>
+        <v>43692</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>142</v>
@@ -7813,25 +8351,25 @@
       <c r="O13">
         <v>101</v>
       </c>
-      <c r="P13" t="e">
+      <c r="P13" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K13,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q13" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.004.QR_LIVE</v>
+      </c>
+      <c r="Q13" t="str">
         <f t="array" aca="1" ref="Q13:T14" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P13))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R13" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S13" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T13" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R13" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S13" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T13" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -7843,21 +8381,21 @@
       <c r="H14" s="2"/>
       <c r="I14" s="3"/>
       <c r="N14" s="7"/>
-      <c r="Q14" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R14" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S14" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T14" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q14" s="37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R14" s="37">
+        <f ca="1"/>
+        <v>1.6633790038974718E-2</v>
+      </c>
+      <c r="S14" s="57">
+        <f ca="1"/>
+        <v>-386706.61906847119</v>
+      </c>
+      <c r="T14" s="57">
+        <f ca="1"/>
+        <v>-379725.40951101558</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -7878,11 +8416,11 @@
       </c>
       <c r="F15" s="2">
         <f ca="1">F13+2</f>
-        <v>43684</v>
+        <v>43691</v>
       </c>
       <c r="G15" s="2">
         <f ca="1">F15+3</f>
-        <v>43687</v>
+        <v>43694</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>142</v>
@@ -7909,25 +8447,25 @@
       <c r="O15">
         <v>101</v>
       </c>
-      <c r="P15" t="e">
+      <c r="P15" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K15,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q15" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.005.QR_LIVE</v>
+      </c>
+      <c r="Q15" t="str">
         <f t="array" aca="1" ref="Q15:T16" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P15))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R15" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S15" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T15" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -7938,21 +8476,21 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
-      <c r="Q16" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R16" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S16" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T16" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q16" s="37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R16" s="37">
+        <f ca="1"/>
+        <v>2.5351217558933454E-2</v>
+      </c>
+      <c r="S16" s="57">
+        <f ca="1"/>
+        <v>-485541.87102598039</v>
+      </c>
+      <c r="T16" s="57">
+        <f ca="1"/>
+        <v>-476776.38995219697</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -7973,11 +8511,11 @@
       </c>
       <c r="F17" s="2">
         <f ca="1">F15+2</f>
-        <v>43686</v>
+        <v>43693</v>
       </c>
       <c r="G17" s="2">
         <f ca="1">F17+3</f>
-        <v>43689</v>
+        <v>43696</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>142</v>
@@ -8004,25 +8542,25 @@
       <c r="O17">
         <v>101</v>
       </c>
-      <c r="P17" t="e">
+      <c r="P17" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K17,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q17" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.006.QR_LIVE</v>
+      </c>
+      <c r="Q17" t="str">
         <f t="array" aca="1" ref="Q17:T18" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P17))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R17" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S17" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T17" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R17" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S17" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T17" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -8031,21 +8569,21 @@
       <c r="G18" s="2"/>
       <c r="I18" s="3"/>
       <c r="N18" s="7"/>
-      <c r="Q18" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R18" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S18" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T18" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q18" s="37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R18" s="37">
+        <f ca="1"/>
+        <v>9.7096967883110147E-2</v>
+      </c>
+      <c r="S18" s="57">
+        <f ca="1"/>
+        <v>587865.63211052795</v>
+      </c>
+      <c r="T18" s="57">
+        <f ca="1"/>
+        <v>577252.90151058184</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -8066,11 +8604,11 @@
       </c>
       <c r="F19" s="2">
         <f ca="1">F17+2</f>
-        <v>43688</v>
+        <v>43695</v>
       </c>
       <c r="G19" s="2">
         <f ca="1">F19+3</f>
-        <v>43691</v>
+        <v>43698</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>142</v>
@@ -8097,25 +8635,25 @@
       <c r="O19">
         <v>101</v>
       </c>
-      <c r="P19" t="e">
+      <c r="P19" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K19,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q19" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.007.QR_LIVE</v>
+      </c>
+      <c r="Q19" t="str">
         <f t="array" aca="1" ref="Q19:T20" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P19))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R19" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S19" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T19" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R19" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S19" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T19" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -8127,21 +8665,21 @@
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
       <c r="N20" s="7"/>
-      <c r="Q20" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R20" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S20" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T20" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q20" s="37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R20" s="37">
+        <f ca="1"/>
+        <v>9.7096967883110147E-2</v>
+      </c>
+      <c r="S20" s="57">
+        <f ca="1"/>
+        <v>685843.23746228265</v>
+      </c>
+      <c r="T20" s="57">
+        <f ca="1"/>
+        <v>673461.71842901211</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -8162,11 +8700,11 @@
       </c>
       <c r="F21" s="2">
         <f ca="1">F19+2</f>
-        <v>43690</v>
+        <v>43697</v>
       </c>
       <c r="G21" s="2">
         <f ca="1">F21+3</f>
-        <v>43693</v>
+        <v>43700</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>142</v>
@@ -8193,25 +8731,25 @@
       <c r="O21">
         <v>101</v>
       </c>
-      <c r="P21" t="e">
+      <c r="P21" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K21,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q21" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.008.QR_LIVE</v>
+      </c>
+      <c r="Q21" t="str">
         <f t="array" aca="1" ref="Q21:T22" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P21))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R21" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S21" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T21" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R21" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S21" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T21" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -8222,21 +8760,21 @@
       <c r="H22" s="2"/>
       <c r="I22" s="3"/>
       <c r="N22" s="7"/>
-      <c r="Q22" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R22" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S22" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T22" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q22" s="37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R22" s="37">
+        <f ca="1"/>
+        <v>8.8262232389927919E-2</v>
+      </c>
+      <c r="S22" s="57">
+        <f ca="1"/>
+        <v>787321.0745362551</v>
+      </c>
+      <c r="T22" s="57">
+        <f ca="1"/>
+        <v>773107.57743196725</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -8257,11 +8795,11 @@
       </c>
       <c r="F23" s="2">
         <f ca="1">F21+2</f>
-        <v>43692</v>
+        <v>43699</v>
       </c>
       <c r="G23" s="2">
         <f ca="1">F23+3</f>
-        <v>43695</v>
+        <v>43702</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>142</v>
@@ -8288,25 +8826,25 @@
       <c r="O23">
         <v>101</v>
       </c>
-      <c r="P23" t="e">
+      <c r="P23" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K23,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q23" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.009.QR_LIVE</v>
+      </c>
+      <c r="Q23" t="str">
         <f t="array" aca="1" ref="Q23:T24" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P23))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R23" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S23" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T23" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R23" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S23" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T23" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -8318,21 +8856,21 @@
       <c r="H24" s="2"/>
       <c r="I24" s="3"/>
       <c r="N24" s="7"/>
-      <c r="Q24" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R24" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S24" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T24" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q24" s="37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R24" s="37">
+        <f ca="1"/>
+        <v>6.9525772005850001E-2</v>
+      </c>
+      <c r="S24" s="57">
+        <f ca="1"/>
+        <v>-893664.56216649467</v>
+      </c>
+      <c r="T24" s="57">
+        <f ca="1"/>
+        <v>-877531.24746506882</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -8353,11 +8891,11 @@
       </c>
       <c r="F25" s="2">
         <f t="shared" ref="F25" ca="1" si="0">F23+2</f>
-        <v>43694</v>
+        <v>43701</v>
       </c>
       <c r="G25" s="2">
         <f ca="1">F25+3</f>
-        <v>43697</v>
+        <v>43704</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>142</v>
@@ -8384,43 +8922,43 @@
       <c r="O25">
         <v>101</v>
       </c>
-      <c r="P25" t="e">
+      <c r="P25" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket(K25,$K$5,Metrics,Currency,$K$2,$K$3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q25" t="e">
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.010.QR_LIVE</v>
+      </c>
+      <c r="Q25" t="str">
         <f t="array" aca="1" ref="Q25:T26" ca="1">TRANSPOSE(_xll.HLV5r3.Financial.Cache.ViewValuationReport(P25))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R25" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S25" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T25" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>YieldToMaturity</v>
+      </c>
+      <c r="R25" t="str">
+        <f ca="1"/>
+        <v>AssetSwapSpread</v>
+      </c>
+      <c r="S25" t="str">
+        <f ca="1"/>
+        <v>NPV</v>
+      </c>
+      <c r="T25" t="str">
+        <f ca="1"/>
+        <v>PandL</v>
       </c>
     </row>
     <row r="26" spans="1:20">
-      <c r="Q26" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R26" s="37" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S26" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T26" s="57" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="Q26" s="37">
+        <f ca="1"/>
+        <v>0.47283841719948799</v>
+      </c>
+      <c r="R26" s="37">
+        <f ca="1"/>
+        <v>0.16112993441480902</v>
+      </c>
+      <c r="S26" s="57">
+        <f ca="1"/>
+        <v>-1038326.4133673233</v>
+      </c>
+      <c r="T26" s="57">
+        <f ca="1"/>
+        <v>-1019581.52015029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started work on a forward curve interpolator.
</commit_message>
<xml_diff>
--- a/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/BondTransactionPricer.xlsx
+++ b/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/BondTransactionPricer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2019\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Product Pricers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E518A6D-FF10-4AEE-9F84-0FD8D96AD2EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DEE0FC-A48A-41B4-ADBF-990769E7A24C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1410" yWindow="465" windowWidth="26370" windowHeight="14820" tabRatio="836" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2192,7 +2192,7 @@
       <c r="F1" s="81"/>
       <c r="G1" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G2:H12, $C$18:$E$41)</f>
-        <v>Market.QR_LIVE.2019-08-25.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-09-01.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H1" s="123"/>
       <c r="I1" s="81"/>
@@ -2222,7 +2222,7 @@
       </c>
       <c r="B3" s="85">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="C3" s="80"/>
       <c r="D3" s="80"/>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="H3" s="85">
         <f ca="1">H6</f>
-        <v>43702</v>
+        <v>43709</v>
       </c>
       <c r="I3" s="84"/>
     </row>
@@ -2243,7 +2243,7 @@
       </c>
       <c r="B4" s="86">
         <f ca="1">B3</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="C4" s="80"/>
       <c r="D4" s="80"/>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="H4" s="86">
         <f ca="1">H3</f>
-        <v>43702</v>
+        <v>43709</v>
       </c>
       <c r="I4" s="84"/>
     </row>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H6" s="88">
         <f ca="1">'BondCurve-BondForward'!G7</f>
-        <v>43702</v>
+        <v>43709</v>
       </c>
       <c r="I6" s="84"/>
     </row>
@@ -2438,7 +2438,7 @@
       <c r="F14" s="84"/>
       <c r="G14" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G15:H25,HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-08-24.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-08-31.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H14" s="123"/>
       <c r="I14" s="84"/>
@@ -2472,7 +2472,7 @@
       </c>
       <c r="H16" s="85">
         <f ca="1">H19</f>
-        <v>43701</v>
+        <v>43708</v>
       </c>
       <c r="I16" s="84"/>
     </row>
@@ -2498,7 +2498,7 @@
       </c>
       <c r="H17" s="86">
         <f ca="1">H16</f>
-        <v>43701</v>
+        <v>43708</v>
       </c>
       <c r="I17" s="84"/>
     </row>
@@ -2551,7 +2551,7 @@
       </c>
       <c r="H19" s="88">
         <f ca="1">'BondCurve-BondForward'!G21</f>
-        <v>43701</v>
+        <v>43708</v>
       </c>
       <c r="I19" s="84"/>
     </row>
@@ -2753,7 +2753,7 @@
       <c r="F27" s="84"/>
       <c r="G27" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G28:H38, HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-08-23.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-08-30.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H27" s="123"/>
       <c r="I27" s="84"/>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="H29" s="85">
         <f ca="1">H32</f>
-        <v>43700</v>
+        <v>43707</v>
       </c>
       <c r="I29" s="84"/>
     </row>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="H30" s="86">
         <f ca="1">H29</f>
-        <v>43700</v>
+        <v>43707</v>
       </c>
       <c r="I30" s="84"/>
     </row>
@@ -2887,7 +2887,7 @@
       </c>
       <c r="H32" s="88">
         <f ca="1">'BondCurve-BondForward'!G35</f>
-        <v>43700</v>
+        <v>43707</v>
       </c>
       <c r="I32" s="84"/>
     </row>
@@ -3089,7 +3089,7 @@
       <c r="F40" s="84"/>
       <c r="G40" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G41:H51, HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-08-22.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-08-29.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H40" s="123"/>
       <c r="I40" s="84"/>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="H42" s="85">
         <f ca="1">H45</f>
-        <v>43699</v>
+        <v>43706</v>
       </c>
       <c r="I42" s="84"/>
     </row>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="H43" s="86">
         <f ca="1">H42</f>
-        <v>43699</v>
+        <v>43706</v>
       </c>
       <c r="I43" s="84"/>
     </row>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="H45" s="88">
         <f ca="1">'BondCurve-BondForward'!G49</f>
-        <v>43699</v>
+        <v>43706</v>
       </c>
       <c r="I45" s="82"/>
     </row>
@@ -3238,7 +3238,7 @@
     <row r="53" spans="7:8" ht="13.5" thickBot="1">
       <c r="G53" s="122" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve( G54:H64, HLInstruments)</f>
-        <v>Market.QR_LIVE.2019-08-21.DiscountCurve.AUD-LIBOR-SENIOR</v>
+        <v>Market.QR_LIVE.2019-08-28.DiscountCurve.AUD-LIBOR-SENIOR</v>
       </c>
       <c r="H53" s="123"/>
     </row>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="H55" s="85">
         <f ca="1">H58</f>
-        <v>43698</v>
+        <v>43705</v>
       </c>
     </row>
     <row r="56" spans="7:8">
@@ -3265,7 +3265,7 @@
       </c>
       <c r="H56" s="86">
         <f ca="1">H55</f>
-        <v>43698</v>
+        <v>43705</v>
       </c>
     </row>
     <row r="57" spans="7:8">
@@ -3282,7 +3282,7 @@
       </c>
       <c r="H58" s="88">
         <f ca="1">'BondCurve-BondForward'!G63</f>
-        <v>43698</v>
+        <v>43705</v>
       </c>
     </row>
     <row r="59" spans="7:8">
@@ -3407,7 +3407,7 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -3416,7 +3416,7 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -3679,7 +3679,7 @@
       </c>
       <c r="C38" s="30">
         <f t="array" aca="1" ref="C38:C42" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B31:B35)</f>
-        <v>2.5000000000000001E-2</v>
+        <v>2.5000000000000012E-2</v>
       </c>
     </row>
     <row r="39" spans="2:3">
@@ -3779,7 +3779,7 @@
       <c r="C2" s="125"/>
       <c r="F2" s="124" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F3:G15, $B$18:$D$21)</f>
-        <v>Market.QR_LIVE.2019-08-25.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-09-01.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G2" s="125"/>
     </row>
@@ -3803,14 +3803,14 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="25">
         <f ca="1">G7</f>
-        <v>43702</v>
+        <v>43709</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -3819,14 +3819,14 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="26">
         <f ca="1">G4</f>
-        <v>43702</v>
+        <v>43709</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="I6" t="str">
         <f ca="1">G6&amp;"."&amp;TEXT(G7,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-25</v>
+        <v>QR_LIVE.2019-09-01</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -3859,11 +3859,11 @@
       </c>
       <c r="G7" s="77">
         <f ca="1">$C$5-1</f>
-        <v>43702</v>
+        <v>43709</v>
       </c>
       <c r="I7" t="str">
         <f ca="1">G20&amp;"."&amp;TEXT(G21,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-24</v>
+        <v>QR_LIVE.2019-08-31</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="I8" t="str">
         <f ca="1">G34&amp;"."&amp;TEXT(G35,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-23</v>
+        <v>QR_LIVE.2019-08-30</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -3899,7 +3899,7 @@
       </c>
       <c r="I9" t="str">
         <f ca="1">G48&amp;"."&amp;TEXT(G49,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-22</v>
+        <v>QR_LIVE.2019-08-29</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -3917,7 +3917,7 @@
       </c>
       <c r="I10" t="str">
         <f ca="1">G62&amp;"."&amp;TEXT(G63,"YYYY-MM-DD")</f>
-        <v>QR_LIVE.2019-08-21</v>
+        <v>QR_LIVE.2019-08-28</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -3990,7 +3990,7 @@
       <c r="D16" s="13"/>
       <c r="F16" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F17:G29, $B$23:$D$26)</f>
-        <v>Market.QR_LIVE.2019-08-24.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-08-31.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G16" s="127"/>
     </row>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="G18" s="25">
         <f ca="1">G21</f>
-        <v>43701</v>
+        <v>43708</v>
       </c>
     </row>
     <row r="19" spans="2:7">
@@ -4044,7 +4044,7 @@
       </c>
       <c r="G19" s="26">
         <f ca="1">G18</f>
-        <v>43701</v>
+        <v>43708</v>
       </c>
     </row>
     <row r="20" spans="2:7">
@@ -4080,7 +4080,7 @@
       </c>
       <c r="G21" s="77">
         <f ca="1">$G$7-1</f>
-        <v>43701</v>
+        <v>43708</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="13.5" thickBot="1">
@@ -4213,7 +4213,7 @@
       </c>
       <c r="F30" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F31:G43, $B$28:$D$31)</f>
-        <v>Market.QR_LIVE.2019-08-23.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-08-30.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G30" s="127"/>
     </row>
@@ -4240,7 +4240,7 @@
       </c>
       <c r="G32" s="25">
         <f ca="1">G35</f>
-        <v>43700</v>
+        <v>43707</v>
       </c>
     </row>
     <row r="33" spans="2:7">
@@ -4258,7 +4258,7 @@
       </c>
       <c r="G33" s="26">
         <f ca="1">G32</f>
-        <v>43700</v>
+        <v>43707</v>
       </c>
     </row>
     <row r="34" spans="2:7">
@@ -4294,7 +4294,7 @@
       </c>
       <c r="G35" s="77">
         <f ca="1">$G$7-2</f>
-        <v>43700</v>
+        <v>43707</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="13.5" thickBot="1">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="F44" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F45:G57, $B$33:$D$36)</f>
-        <v>Market.QR_LIVE.2019-08-22.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-08-29.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G44" s="127"/>
     </row>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="G46" s="25">
         <f ca="1">G49</f>
-        <v>43699</v>
+        <v>43706</v>
       </c>
     </row>
     <row r="47" spans="2:7">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="G47" s="26">
         <f ca="1">G46</f>
-        <v>43699</v>
+        <v>43706</v>
       </c>
     </row>
     <row r="48" spans="2:7">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="G49" s="77">
         <f ca="1">$G$7-3</f>
-        <v>43699</v>
+        <v>43706</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="13.5" thickBot="1">
@@ -4522,7 +4522,7 @@
     <row r="52" spans="2:7">
       <c r="B52" s="73">
         <f t="array" aca="1" ref="B52:C56" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="C52" s="30">
         <f ca="1"/>
@@ -4538,7 +4538,7 @@
     <row r="53" spans="2:7">
       <c r="B53" s="74">
         <f ca="1"/>
-        <v>43705</v>
+        <v>43712</v>
       </c>
       <c r="C53" s="31">
         <f ca="1"/>
@@ -4554,7 +4554,7 @@
     <row r="54" spans="2:7">
       <c r="B54" s="74">
         <f ca="1"/>
-        <v>43738</v>
+        <v>43742</v>
       </c>
       <c r="C54" s="31">
         <f ca="1"/>
@@ -4570,7 +4570,7 @@
     <row r="55" spans="2:7">
       <c r="B55" s="74">
         <f ca="1"/>
-        <v>43766</v>
+        <v>43773</v>
       </c>
       <c r="C55" s="31">
         <f ca="1"/>
@@ -4613,14 +4613,14 @@
       </c>
       <c r="F58" s="126" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateCurve(F59:G71, $B$38:$D$41)</f>
-        <v>Market.QR_LIVE.2019-08-21.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
+        <v>Market.QR_LIVE.2019-08-28.BondCurve.AUD-Govt:WATC:Fixed:7-15/10/2019</v>
       </c>
       <c r="G58" s="127"/>
     </row>
     <row r="59" spans="2:7" ht="13.5" thickBot="1">
       <c r="B59" s="73">
         <f ca="1">B52</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="C59" s="30">
         <f t="array" aca="1" ref="C59:C63" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B52:B56)</f>
@@ -4636,7 +4636,7 @@
     <row r="60" spans="2:7">
       <c r="B60" s="74">
         <f t="shared" ref="B60:B63" ca="1" si="0">B53</f>
-        <v>43705</v>
+        <v>43712</v>
       </c>
       <c r="C60" s="31">
         <f ca="1"/>
@@ -4647,13 +4647,13 @@
       </c>
       <c r="G60" s="25">
         <f ca="1">G63</f>
-        <v>43698</v>
+        <v>43705</v>
       </c>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43738</v>
+        <v>43742</v>
       </c>
       <c r="C61" s="31">
         <f ca="1"/>
@@ -4664,13 +4664,13 @@
       </c>
       <c r="G61" s="26">
         <f ca="1">G60</f>
-        <v>43698</v>
+        <v>43705</v>
       </c>
     </row>
     <row r="62" spans="2:7">
       <c r="B62" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43766</v>
+        <v>43773</v>
       </c>
       <c r="C62" s="31">
         <f ca="1"/>
@@ -4698,7 +4698,7 @@
       </c>
       <c r="G63" s="77">
         <f ca="1">$G$7-4</f>
-        <v>43698</v>
+        <v>43705</v>
       </c>
     </row>
     <row r="64" spans="2:7">
@@ -4816,7 +4816,7 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -4825,7 +4825,7 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -5033,7 +5033,7 @@
     <row r="32" spans="2:4">
       <c r="B32" s="73">
         <f t="array" aca="1" ref="B32:C36" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="C32" s="30">
         <f ca="1"/>
@@ -5043,7 +5043,7 @@
     <row r="33" spans="2:3">
       <c r="B33" s="74">
         <f ca="1"/>
-        <v>43704</v>
+        <v>43711</v>
       </c>
       <c r="C33" s="31">
         <f ca="1"/>
@@ -5053,17 +5053,17 @@
     <row r="34" spans="2:3">
       <c r="B34" s="74">
         <f ca="1"/>
-        <v>43735</v>
+        <v>43741</v>
       </c>
       <c r="C34" s="31">
         <f ca="1"/>
-        <v>0.99563499344803497</v>
+        <v>0.99577082359720903</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="74">
         <f ca="1"/>
-        <v>43766</v>
+        <v>43773</v>
       </c>
       <c r="C35" s="31">
         <f ca="1"/>
@@ -5073,11 +5073,11 @@
     <row r="36" spans="2:3" ht="13.5" thickBot="1">
       <c r="B36" s="75">
         <f ca="1"/>
-        <v>43796</v>
+        <v>43802</v>
       </c>
       <c r="C36" s="32">
         <f ca="1"/>
-        <v>0.98741884969798999</v>
+        <v>0.98755244716108004</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="13.5" thickBot="1"/>
@@ -5089,7 +5089,7 @@
     <row r="39" spans="2:3">
       <c r="B39" s="73">
         <f ca="1">B32</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="C39" s="30">
         <f t="array" aca="1" ref="C39:C43" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B32:B36)</f>
@@ -5099,7 +5099,7 @@
     <row r="40" spans="2:3">
       <c r="B40" s="74">
         <f t="shared" ref="B40:B43" ca="1" si="0">B33</f>
-        <v>43704</v>
+        <v>43711</v>
       </c>
       <c r="C40" s="31">
         <f ca="1"/>
@@ -5109,17 +5109,17 @@
     <row r="41" spans="2:3">
       <c r="B41" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43735</v>
+        <v>43741</v>
       </c>
       <c r="C41" s="31">
         <f ca="1"/>
-        <v>0.99563499344803497</v>
+        <v>0.99577082359720903</v>
       </c>
     </row>
     <row r="42" spans="2:3">
       <c r="B42" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43766</v>
+        <v>43773</v>
       </c>
       <c r="C42" s="31">
         <f ca="1"/>
@@ -5129,11 +5129,11 @@
     <row r="43" spans="2:3" ht="13.5" thickBot="1">
       <c r="B43" s="75">
         <f t="shared" ca="1" si="0"/>
-        <v>43796</v>
+        <v>43802</v>
       </c>
       <c r="C43" s="32">
         <f ca="1"/>
-        <v>0.9874188496979901</v>
+        <v>0.98755244716108015</v>
       </c>
     </row>
     <row r="45" spans="2:3">
@@ -5221,14 +5221,14 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">C5</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="25">
         <f ca="1">G5</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -5237,14 +5237,14 @@
       </c>
       <c r="C5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="26">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -5452,7 +5452,7 @@
       </c>
       <c r="G20" s="25">
         <f ca="1">G21</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -5471,7 +5471,7 @@
       </c>
       <c r="G21" s="26">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="22" spans="2:7">
@@ -5572,7 +5572,7 @@
       </c>
       <c r="C28" s="65">
         <f ca="1"/>
-        <v>5.000658682216922E-2</v>
+        <v>5.0006605708307825E-2</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>35</v>
@@ -5604,7 +5604,7 @@
       </c>
       <c r="C30" s="65">
         <f ca="1"/>
-        <v>5.0006791423151439E-2</v>
+        <v>5.0006782017395265E-2</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>38</v>
@@ -5651,7 +5651,7 @@
     <row r="34" spans="2:7" ht="13.5" thickBot="1">
       <c r="B34" s="73">
         <f t="array" aca="1" ref="B34:C38" ca="1">_xll.HLV5r3.Financial.Cache.GetTermCurve(B2)</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="C34" s="64">
         <f ca="1"/>
@@ -5666,7 +5666,7 @@
     <row r="35" spans="2:7" ht="13.5" thickBot="1">
       <c r="B35" s="74">
         <f ca="1"/>
-        <v>43704</v>
+        <v>43711</v>
       </c>
       <c r="C35" s="65">
         <f ca="1"/>
@@ -5682,24 +5682,24 @@
     <row r="36" spans="2:7">
       <c r="B36" s="74">
         <f ca="1"/>
-        <v>43735</v>
+        <v>43741</v>
       </c>
       <c r="C36" s="65">
         <f ca="1"/>
-        <v>0.99563443844231203</v>
+        <v>0.99577028484175101</v>
       </c>
       <c r="F36" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G36" s="25">
         <f ca="1">G37</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="74">
         <f ca="1"/>
-        <v>43766</v>
+        <v>43773</v>
       </c>
       <c r="C37" s="65">
         <f ca="1"/>
@@ -5710,17 +5710,17 @@
       </c>
       <c r="G37" s="26">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="13.5" thickBot="1">
       <c r="B38" s="75">
         <f ca="1"/>
-        <v>43796</v>
+        <v>43802</v>
       </c>
       <c r="C38" s="66">
         <f ca="1"/>
-        <v>0.987417180468115</v>
+        <v>0.98755079791521005</v>
       </c>
       <c r="F38" s="22" t="s">
         <v>26</v>
@@ -5753,7 +5753,7 @@
     <row r="41" spans="2:7">
       <c r="B41" s="73">
         <f ca="1">B34</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="C41" s="64">
         <f t="array" aca="1" ref="C41:C45" ca="1">_xll.HLV5r3.Financial.Cache.GetValues(B2,B34:B38)</f>
@@ -5769,7 +5769,7 @@
     <row r="42" spans="2:7">
       <c r="B42" s="74">
         <f t="shared" ref="B42:B45" ca="1" si="0">B35</f>
-        <v>43704</v>
+        <v>43711</v>
       </c>
       <c r="C42" s="65">
         <f ca="1"/>
@@ -5785,11 +5785,11 @@
     <row r="43" spans="2:7">
       <c r="B43" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43735</v>
+        <v>43741</v>
       </c>
       <c r="C43" s="65">
         <f ca="1"/>
-        <v>5.0216290738325703E-2</v>
+        <v>5.0219744702932403E-2</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>34</v>
@@ -5801,7 +5801,7 @@
     <row r="44" spans="2:7">
       <c r="B44" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>43766</v>
+        <v>43773</v>
       </c>
       <c r="C44" s="65">
         <f ca="1"/>
@@ -5817,11 +5817,11 @@
     <row r="45" spans="2:7" ht="13.5" thickBot="1">
       <c r="B45" s="75">
         <f t="shared" ca="1" si="0"/>
-        <v>43796</v>
+        <v>43802</v>
       </c>
       <c r="C45" s="66">
         <f ca="1"/>
-        <v>5.0007524364018799E-2</v>
+        <v>5.0010925007097001E-2</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>37</v>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="G52" s="25">
         <f ca="1">G53</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="53" spans="2:7">
@@ -5902,7 +5902,7 @@
       </c>
       <c r="G53" s="26">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
     </row>
     <row r="54" spans="2:7">
@@ -6018,10 +6018,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:V45"/>
+  <dimension ref="B1:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6035,17 +6035,22 @@
     <col min="7" max="7" width="3.7109375" customWidth="1"/>
     <col min="8" max="8" width="84.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22">
+    <row r="1" spans="2:25">
       <c r="F1" t="str">
         <f t="array" ref="F1:F13">_xll.HLV5r3.Financial.Cache.SupportedBondMetrics()</f>
         <v>DirtyPrice</v>
@@ -6059,65 +6064,77 @@
         <v>QR_LIVE</v>
       </c>
       <c r="K1" t="str">
-        <f t="array" aca="1" ref="K1:V11" ca="1">_xll.HLV5r3.Financial.Cache.ViewExpectedCashFlows(B22,C18,E3:E7,C27,$I$1,C16)</f>
+        <f t="array" aca="1" ref="K1:Y11" ca="1">_xll.HLV5r3.Financial.Cache.ViewExpectedCashFlows(B22,C18,E3:E7,C27,$I$1,C16)</f>
         <v>Trade.SpreadSheet.bondTransaction.testtrade_001</v>
       </c>
       <c r="L1" t="str">
         <f ca="1"/>
         <v>PrincipalExchange</v>
       </c>
-      <c r="M1">
-        <f ca="1"/>
-        <v>43708</v>
+      <c r="M1" s="2">
+        <f ca="1"/>
+        <v>43715</v>
       </c>
       <c r="N1" t="str">
         <f ca="1"/>
         <v>AUD</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="3">
         <f ca="1"/>
         <v>-101000000</v>
       </c>
-      <c r="P1" t="str">
+      <c r="P1">
+        <f ca="1"/>
+        <v>-101000000</v>
+      </c>
+      <c r="Q1" t="str">
         <f ca="1"/>
         <v>DiscountedCashflow</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <f ca="1"/>
         <v>0.99931544357534796</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <f ca="1"/>
         <v>-100930859.80111015</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <f ca="1"/>
         <v>1.3698630136986301E-2</v>
       </c>
-      <c r="T1" t="b">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
       <c r="U1" t="b">
         <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="V1" t="b">
+        <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="V1" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="2" spans="2:22">
+      <c r="W1" t="str">
+        <f ca="1"/>
+        <v>Party1</v>
+      </c>
+      <c r="X1" t="str">
+        <f ca="1"/>
+        <v>Party2</v>
+      </c>
+      <c r="Y1" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="2" spans="2:25">
       <c r="F2" t="str">
         <v>CleanPrice</v>
       </c>
       <c r="H2" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I2,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-25</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-09-01</v>
       </c>
       <c r="I2" t="str">
         <f ca="1">'BondCurve-BondForward'!I6</f>
-        <v>QR_LIVE.2019-08-25</v>
+        <v>QR_LIVE.2019-09-01</v>
       </c>
       <c r="K2" t="str">
         <f ca="1"/>
@@ -6127,7 +6144,7 @@
         <f ca="1"/>
         <v>PrincipalExchange</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="2">
         <f ca="1"/>
         <v>43753</v>
       </c>
@@ -6135,40 +6152,52 @@
         <f ca="1"/>
         <v>AUD</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="3">
         <f ca="1"/>
         <v>100000000</v>
       </c>
-      <c r="P2" t="str">
+      <c r="P2">
+        <f ca="1"/>
+        <v>100000000</v>
+      </c>
+      <c r="Q2" t="str">
         <f ca="1"/>
         <v>DiscountedCashflow</v>
       </c>
-      <c r="Q2">
-        <f ca="1"/>
-        <v>0.99319547997258495</v>
-      </c>
       <c r="R2">
         <f ca="1"/>
-        <v>99319547.997258514</v>
+        <v>0.99414254148981696</v>
       </c>
       <c r="S2">
         <f ca="1"/>
-        <v>0.13698630136986301</v>
-      </c>
-      <c r="T2" t="b">
-        <f ca="1"/>
-        <v>0</v>
+        <v>99414254.14898169</v>
+      </c>
+      <c r="T2">
+        <f ca="1"/>
+        <v>0.117808219178082</v>
       </c>
       <c r="U2" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="V2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="2:22">
+      <c r="V2" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="W2" t="str">
+        <f ca="1"/>
+        <v>WATC</v>
+      </c>
+      <c r="X2" t="str">
+        <f ca="1"/>
+        <v>Party1</v>
+      </c>
+      <c r="Y2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -6183,11 +6212,11 @@
       </c>
       <c r="H3" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I3,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-24</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-31</v>
       </c>
       <c r="I3" t="str">
         <f ca="1">'BondCurve-BondForward'!I7</f>
-        <v>QR_LIVE.2019-08-24</v>
+        <v>QR_LIVE.2019-08-31</v>
       </c>
       <c r="K3" t="str">
         <f ca="1"/>
@@ -6197,7 +6226,7 @@
         <f ca="1"/>
         <v>Coupon</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="2">
         <f ca="1"/>
         <v>43570</v>
       </c>
@@ -6205,40 +6234,52 @@
         <f ca="1"/>
         <v>AUD</v>
       </c>
-      <c r="O3">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" t="str">
+      <c r="O3" s="3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f ca="1"/>
+        <v>3490410.9589041071</v>
+      </c>
+      <c r="Q3" t="str">
         <f ca="1"/>
         <v>FixedRateRateCoupon</v>
       </c>
-      <c r="Q3">
-        <f ca="1"/>
-        <v>1.0183848891398799</v>
-      </c>
       <c r="R3">
         <f ca="1"/>
-        <v>0</v>
+        <v>1.01936182400197</v>
       </c>
       <c r="S3">
         <f ca="1"/>
-        <v>-0.36438356164383601</v>
-      </c>
-      <c r="T3" t="b">
-        <f ca="1"/>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f ca="1"/>
+        <v>-0.38356164383561597</v>
       </c>
       <c r="U3" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="V3" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22">
+      <c r="V3" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="W3" t="str">
+        <f ca="1"/>
+        <v>Not specified</v>
+      </c>
+      <c r="X3" t="str">
+        <f ca="1"/>
+        <v>Not specified</v>
+      </c>
+      <c r="Y3" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -6253,11 +6294,11 @@
       </c>
       <c r="H4" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I4,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-23</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-30</v>
       </c>
       <c r="I4" t="str">
         <f ca="1">'BondCurve-BondForward'!I8</f>
-        <v>QR_LIVE.2019-08-23</v>
+        <v>QR_LIVE.2019-08-30</v>
       </c>
       <c r="K4" t="str">
         <f ca="1"/>
@@ -6267,7 +6308,7 @@
         <f ca="1"/>
         <v>Coupon</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
         <f ca="1"/>
         <v>43753</v>
       </c>
@@ -6275,40 +6316,52 @@
         <f ca="1"/>
         <v>AUD</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="3">
         <f ca="1"/>
         <v>3509589.0410958929</v>
       </c>
-      <c r="P4" t="str">
+      <c r="P4">
+        <f ca="1"/>
+        <v>3509589.0410958929</v>
+      </c>
+      <c r="Q4" t="str">
         <f ca="1"/>
         <v>FixedRateRateCoupon</v>
       </c>
-      <c r="Q4">
-        <f ca="1"/>
-        <v>0.99319547997258495</v>
-      </c>
       <c r="R4">
         <f ca="1"/>
-        <v>3485707.9721777597</v>
+        <v>0.99414254148981696</v>
       </c>
       <c r="S4">
         <f ca="1"/>
-        <v>0.13698630136986301</v>
-      </c>
-      <c r="T4" t="b">
-        <f ca="1"/>
-        <v>0</v>
+        <v>3489031.7688998813</v>
+      </c>
+      <c r="T4">
+        <f ca="1"/>
+        <v>0.117808219178082</v>
       </c>
       <c r="U4" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="V4" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="2:22">
+      <c r="V4" t="b">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="W4" t="str">
+        <f ca="1"/>
+        <v>Not specified</v>
+      </c>
+      <c r="X4" t="str">
+        <f ca="1"/>
+        <v>Not specified</v>
+      </c>
+      <c r="Y4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -6323,11 +6376,11 @@
       </c>
       <c r="H5" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I5,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-22</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-29</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">'BondCurve-BondForward'!I9</f>
-        <v>QR_LIVE.2019-08-22</v>
+        <v>QR_LIVE.2019-08-29</v>
       </c>
       <c r="K5" t="e">
         <f ca="1"/>
@@ -6377,8 +6430,20 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="6" spans="2:22">
+      <c r="W5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y5" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -6393,11 +6458,11 @@
       </c>
       <c r="H6" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.ValueTradeFromMarket($B$22,$C$18,$E$3:$E$7,"AUD",I6,$C$10)</f>
-        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-21</v>
+        <v>ValuationReport.LOCAL_USER.SpreadSheet.bondTransaction.testtrade_001.QR_LIVE.2019-08-28</v>
       </c>
       <c r="I6" t="str">
         <f ca="1">'BondCurve-BondForward'!I10</f>
-        <v>QR_LIVE.2019-08-21</v>
+        <v>QR_LIVE.2019-08-28</v>
       </c>
       <c r="K6" t="e">
         <f ca="1"/>
@@ -6447,8 +6512,20 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="7" spans="2:22">
+      <c r="W6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y6" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25">
       <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
@@ -6505,8 +6582,20 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="8" spans="2:22">
+      <c r="W7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y7" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25">
       <c r="B8" t="s">
         <v>141</v>
       </c>
@@ -6566,8 +6655,20 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="9" spans="2:22">
+      <c r="W8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y8" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -6625,14 +6726,26 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="10" spans="2:22">
+      <c r="W9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y9" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="F10" t="str">
         <v>AssetSwapSpread</v>
@@ -6685,14 +6798,26 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="11" spans="2:22">
+      <c r="W10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y10" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25">
       <c r="B11" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="2">
         <f ca="1">C10+5</f>
-        <v>43708</v>
+        <v>43715</v>
       </c>
       <c r="F11" t="str">
         <v>ZSpread</v>
@@ -6745,8 +6870,20 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="12" spans="2:22">
+      <c r="W11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y11" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -6757,7 +6894,7 @@
         <v>YieldToMaturity</v>
       </c>
     </row>
-    <row r="13" spans="2:22">
+    <row r="13" spans="2:25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -6771,7 +6908,7 @@
         <v>PandL</v>
       </c>
     </row>
-    <row r="14" spans="2:22">
+    <row r="14" spans="2:25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -6782,7 +6919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:22">
+    <row r="15" spans="2:25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -6790,13 +6927,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:22">
+    <row r="16" spans="2:25">
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="2">
         <f ca="1">C10</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="E16" t="str">
         <f t="array" aca="1" ref="E16:F22" ca="1">_xll.HLV5r3.Financial.Cache.ViewValuationReport(H1)</f>
@@ -6804,7 +6941,7 @@
       </c>
       <c r="F16" s="60">
         <f ca="1"/>
-        <v>1.0622265512299201E-3</v>
+        <v>1.1281164084270599E-3</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -6820,7 +6957,7 @@
       </c>
       <c r="F17" s="60">
         <f ca="1"/>
-        <v>-0.12454490731241699</v>
+        <v>-0.12458892121023411</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -6836,7 +6973,7 @@
       </c>
       <c r="F18" s="115">
         <f ca="1"/>
-        <v>108954135.48004666</v>
+        <v>109060210.50277404</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -6852,7 +6989,7 @@
       </c>
       <c r="F19" s="115">
         <f ca="1"/>
-        <v>106987187.891278</v>
+        <v>106988713.854918</v>
       </c>
     </row>
     <row r="20" spans="2:6">
@@ -6868,7 +7005,7 @@
       </c>
       <c r="F20">
         <f ca="1"/>
-        <v>1.0698718789127799</v>
+        <v>1.0698871385491799</v>
       </c>
     </row>
     <row r="21" spans="2:6">
@@ -6884,7 +7021,7 @@
       </c>
       <c r="F21">
         <f ca="1"/>
-        <v>10057.556785162775</v>
+        <v>10067.17635783548</v>
       </c>
     </row>
     <row r="22" spans="2:6">
@@ -6899,7 +7036,7 @@
       </c>
       <c r="F22">
         <f ca="1"/>
-        <v>5089664.6875904994</v>
+        <v>5095118.1129413005</v>
       </c>
     </row>
     <row r="24" spans="2:6">
@@ -7260,7 +7397,7 @@
       </c>
       <c r="C10" s="2">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="E10" s="114" t="s">
         <v>140</v>
@@ -7278,7 +7415,7 @@
       </c>
       <c r="C11" s="2">
         <f ca="1">C10+5</f>
-        <v>43708</v>
+        <v>43715</v>
       </c>
       <c r="H11" t="str">
         <v>ZSpread</v>
@@ -7334,7 +7471,7 @@
       </c>
       <c r="C16" s="2">
         <f ca="1">C10</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="E16" s="61" t="str">
         <f t="array" ref="E16:F22">_xll.HLV5r3.Financial.Cache.ViewValuationReport(E27)</f>
@@ -7508,7 +7645,7 @@
       </c>
       <c r="H29" s="1" t="str">
         <f t="array" aca="1" ref="H29:H33" ca="1">Markets</f>
-        <v>QR_LIVE.2019-08-25</v>
+        <v>QR_LIVE.2019-09-01</v>
       </c>
     </row>
     <row r="30" spans="2:8">
@@ -7522,7 +7659,7 @@
       </c>
       <c r="H30" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-08-24</v>
+        <v>QR_LIVE.2019-08-31</v>
       </c>
     </row>
     <row r="31" spans="2:8">
@@ -7536,7 +7673,7 @@
       </c>
       <c r="H31" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-08-23</v>
+        <v>QR_LIVE.2019-08-30</v>
       </c>
     </row>
     <row r="32" spans="2:8">
@@ -7557,7 +7694,7 @@
       </c>
       <c r="H32" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-08-22</v>
+        <v>QR_LIVE.2019-08-29</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -7577,7 +7714,7 @@
       </c>
       <c r="H33" t="str">
         <f ca="1"/>
-        <v>QR_LIVE.2019-08-21</v>
+        <v>QR_LIVE.2019-08-28</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -7931,7 +8068,7 @@
       </c>
       <c r="K3" s="50">
         <f ca="1">TODAY()</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>21</v>
@@ -8040,11 +8177,11 @@
       </c>
       <c r="F7" s="2">
         <f ca="1">TODAY()-20</f>
-        <v>43683</v>
+        <v>43690</v>
       </c>
       <c r="G7" s="2">
         <f ca="1">F7+3</f>
-        <v>43686</v>
+        <v>43693</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>142</v>
@@ -8099,15 +8236,15 @@
       </c>
       <c r="R8" s="37">
         <f ca="1"/>
-        <v>0.14928664798605062</v>
+        <v>0.11900111569850146</v>
       </c>
       <c r="S8" s="57">
         <f ca="1"/>
-        <v>95392.978256669478</v>
+        <v>96985.222627684518</v>
       </c>
       <c r="T8" s="57">
         <f ca="1"/>
-        <v>93670.850062629703</v>
+        <v>95143.079075616901</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -8128,11 +8265,11 @@
       </c>
       <c r="F9" s="2">
         <f ca="1">F7+2</f>
-        <v>43685</v>
+        <v>43692</v>
       </c>
       <c r="G9" s="2">
         <f ca="1">F9+3</f>
-        <v>43688</v>
+        <v>43695</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>142</v>
@@ -8195,15 +8332,15 @@
       </c>
       <c r="R10" s="37">
         <f ca="1"/>
-        <v>0.13204488198804987</v>
+        <v>0.10148825950699564</v>
       </c>
       <c r="S10" s="57">
         <f ca="1"/>
-        <v>192493.7092904264</v>
+        <v>195706.70285321036</v>
       </c>
       <c r="T10" s="57">
         <f ca="1"/>
-        <v>189018.6228637044</v>
+        <v>191989.4371606682</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -8224,11 +8361,11 @@
       </c>
       <c r="F11" s="2">
         <f ca="1">F9+2</f>
-        <v>43687</v>
+        <v>43694</v>
       </c>
       <c r="G11" s="2">
         <f ca="1">F11+3</f>
-        <v>43690</v>
+        <v>43697</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>142</v>
@@ -8291,15 +8428,15 @@
       </c>
       <c r="R12" s="37">
         <f ca="1"/>
-        <v>0.12771037962458848</v>
+        <v>9.7085606289113002E-2</v>
       </c>
       <c r="S12" s="57">
         <f ca="1"/>
-        <v>289384.54597750399</v>
+        <v>294214.78529712814</v>
       </c>
       <c r="T12" s="57">
         <f ca="1"/>
-        <v>284160.29053800664</v>
+        <v>288626.45075529092</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -8320,11 +8457,11 @@
       </c>
       <c r="F13" s="2">
         <f ca="1">F11+2</f>
-        <v>43689</v>
+        <v>43696</v>
       </c>
       <c r="G13" s="2">
         <f ca="1">F13+3</f>
-        <v>43692</v>
+        <v>43699</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>142</v>
@@ -8387,15 +8524,15 @@
       </c>
       <c r="R14" s="37">
         <f ca="1"/>
-        <v>1.6633790038974718E-2</v>
+        <v>4.7326866226654399E-2</v>
       </c>
       <c r="S14" s="57">
         <f ca="1"/>
-        <v>-386706.61906847119</v>
+        <v>-393161.30209335039</v>
       </c>
       <c r="T14" s="57">
         <f ca="1"/>
-        <v>-379725.40951101558</v>
+        <v>-385693.57105195121</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -8416,11 +8553,11 @@
       </c>
       <c r="F15" s="2">
         <f ca="1">F13+2</f>
-        <v>43691</v>
+        <v>43698</v>
       </c>
       <c r="G15" s="2">
         <f ca="1">F15+3</f>
-        <v>43694</v>
+        <v>43701</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>142</v>
@@ -8482,15 +8619,15 @@
       </c>
       <c r="R16" s="37">
         <f ca="1"/>
-        <v>2.5351217558933454E-2</v>
+        <v>5.6181356801150772E-2</v>
       </c>
       <c r="S16" s="57">
         <f ca="1"/>
-        <v>-485541.87102598039</v>
+        <v>-493646.25486179156</v>
       </c>
       <c r="T16" s="57">
         <f ca="1"/>
-        <v>-476776.38995219697</v>
+        <v>-484269.90616909502</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -8511,11 +8648,11 @@
       </c>
       <c r="F17" s="2">
         <f ca="1">F15+2</f>
-        <v>43693</v>
+        <v>43700</v>
       </c>
       <c r="G17" s="2">
         <f ca="1">F17+3</f>
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>142</v>
@@ -8575,15 +8712,15 @@
       </c>
       <c r="R18" s="37">
         <f ca="1"/>
-        <v>9.7096967883110147E-2</v>
+        <v>6.5990863591521343E-2</v>
       </c>
       <c r="S18" s="57">
         <f ca="1"/>
-        <v>587865.63211052795</v>
+        <v>597677.94493215554</v>
       </c>
       <c r="T18" s="57">
         <f ca="1"/>
-        <v>577252.90151058184</v>
+        <v>586325.61163189134</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -8604,11 +8741,11 @@
       </c>
       <c r="F19" s="2">
         <f ca="1">F17+2</f>
-        <v>43695</v>
+        <v>43702</v>
       </c>
       <c r="G19" s="2">
         <f ca="1">F19+3</f>
-        <v>43698</v>
+        <v>43705</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>142</v>
@@ -8671,15 +8808,15 @@
       </c>
       <c r="R20" s="37">
         <f ca="1"/>
-        <v>9.7096967883110147E-2</v>
+        <v>6.5990863591521343E-2</v>
       </c>
       <c r="S20" s="57">
         <f ca="1"/>
-        <v>685843.23746228265</v>
+        <v>697290.93575418147</v>
       </c>
       <c r="T20" s="57">
         <f ca="1"/>
-        <v>673461.71842901211</v>
+        <v>684046.54690387333</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -8700,11 +8837,11 @@
       </c>
       <c r="F21" s="2">
         <f ca="1">F19+2</f>
-        <v>43697</v>
+        <v>43704</v>
       </c>
       <c r="G21" s="2">
         <f ca="1">F21+3</f>
-        <v>43700</v>
+        <v>43707</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>142</v>
@@ -8766,15 +8903,15 @@
       </c>
       <c r="R22" s="37">
         <f ca="1"/>
-        <v>8.8262232389927919E-2</v>
+        <v>5.7017220624783135E-2</v>
       </c>
       <c r="S22" s="57">
         <f ca="1"/>
-        <v>787321.0745362551</v>
+        <v>800462.58214008308</v>
       </c>
       <c r="T22" s="57">
         <f ca="1"/>
-        <v>773107.57743196725</v>
+        <v>785258.54440722719</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -8795,11 +8932,11 @@
       </c>
       <c r="F23" s="2">
         <f ca="1">F21+2</f>
-        <v>43699</v>
+        <v>43706</v>
       </c>
       <c r="G23" s="2">
         <f ca="1">F23+3</f>
-        <v>43702</v>
+        <v>43709</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>142</v>
@@ -8862,15 +8999,15 @@
       </c>
       <c r="R24" s="37">
         <f ca="1"/>
-        <v>6.9525772005850001E-2</v>
+        <v>0.10105046240451337</v>
       </c>
       <c r="S24" s="57">
         <f ca="1"/>
-        <v>-893664.56216649467</v>
+        <v>-908581.09370466077</v>
       </c>
       <c r="T24" s="57">
         <f ca="1"/>
-        <v>-877531.24746506882</v>
+        <v>-891323.44601410627</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -8891,11 +9028,11 @@
       </c>
       <c r="F25" s="2">
         <f t="shared" ref="F25" ca="1" si="0">F23+2</f>
-        <v>43701</v>
+        <v>43708</v>
       </c>
       <c r="G25" s="2">
         <f ca="1">F25+3</f>
-        <v>43704</v>
+        <v>43711</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>142</v>
@@ -8950,15 +9087,15 @@
       </c>
       <c r="R26" s="37">
         <f ca="1"/>
-        <v>0.16112993441480902</v>
+        <v>0.17832535650914855</v>
       </c>
       <c r="S26" s="57">
         <f ca="1"/>
-        <v>-1038326.4133673233</v>
+        <v>-1047840.4423979232</v>
       </c>
       <c r="T26" s="57">
         <f ca="1"/>
-        <v>-1019581.52015029</v>
+        <v>-1027937.69368775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>